<commit_message>
Transfered data from .xlsx to .docx
</commit_message>
<xml_diff>
--- a/Lab1/Auswertung Final.xlsx
+++ b/Lab1/Auswertung Final.xlsx
@@ -314,7 +314,7 @@
     <numFmt numFmtId="168" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -626,7 +626,14 @@
   </cellStyles>
   <dxfs count="159">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -635,7 +642,17 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -644,13 +661,46 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -741,6 +791,63 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -890,48 +997,6 @@
       <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
@@ -954,68 +1019,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
@@ -1082,9 +1085,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
@@ -5645,6 +5645,7 @@
         <c:crossAx val="270221696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="270221696"/>
@@ -6265,6 +6266,7 @@
         <c:crossAx val="270221696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="270221696"/>
@@ -6885,6 +6887,7 @@
         <c:crossAx val="270221696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="270221696"/>
@@ -7505,6 +7508,7 @@
         <c:crossAx val="270221696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="270221696"/>
@@ -8125,6 +8129,7 @@
         <c:crossAx val="270221696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="270221696"/>
@@ -9409,6 +9414,7 @@
         <c:crossAx val="270221696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="270221696"/>
@@ -10029,6 +10035,7 @@
         <c:crossAx val="270221696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="270221696"/>
@@ -11969,6 +11976,7 @@
         <c:crossAx val="270221696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="270221696"/>
@@ -42852,31 +42860,31 @@
   <tableColumns count="9">
     <tableColumn id="1" name="Posten" totalsRowLabel="Gesamt"/>
     <tableColumn id="9" name="0" totalsRowLabel="0"/>
-    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="151" totalsRowDxfId="64">
+    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="151" totalsRowDxfId="150">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!B2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!B2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!B12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="150" totalsRowDxfId="63">
+    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="149" totalsRowDxfId="148">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!C2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!C2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!C12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="149" totalsRowDxfId="62">
+    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="147" totalsRowDxfId="146">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!D2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!D2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!D12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="148" totalsRowDxfId="61">
+    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="145" totalsRowDxfId="144">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!E2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!E2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!E12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="147" totalsRowDxfId="60">
+    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="143" totalsRowDxfId="142">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!F2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!F2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!F12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="146" totalsRowDxfId="59">
+    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="141" totalsRowDxfId="140">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!G2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!G12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="145" totalsRowDxfId="58">
+    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="139" totalsRowDxfId="138">
       <calculatedColumnFormula>SUM('Budgetierte Kosten'!$B2:'Budgetierte Kosten'!H2)*'Budgetierte Kosten'!$B$14*'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
       <totalsRowFormula>SUM('Budgetierte Kosten'!$B12:'Budgetierte Kosten'!H12)</totalsRowFormula>
     </tableColumn>
@@ -42889,7 +42897,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="EAC" displayName="EAC" ref="B109:J117" totalsRowCount="1">
   <autoFilter ref="B109:J116"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="119">
+    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="31">
       <calculatedColumnFormula>B97</calculatedColumnFormula>
       <totalsRowFormula>ETC[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
@@ -42897,31 +42905,31 @@
       <calculatedColumnFormula>C97</calculatedColumnFormula>
       <totalsRowFormula>ETC[[#Totals],[0 '[k €']]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="1 [k €]" totalsRowFunction="custom" dataDxfId="118" totalsRowDxfId="22">
+    <tableColumn id="2" name="1 [k €]" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="29">
       <calculatedColumnFormula>IF(D69=$M$70,$M$70,'Budgetierte Kosten'!$P2/(D69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[1]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2 [k €]" totalsRowFunction="custom" dataDxfId="117" totalsRowDxfId="21">
+    <tableColumn id="3" name="2 [k €]" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="27">
       <calculatedColumnFormula>IF(E69=$M$70,$M$70,$E$92/(E69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[2]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3 [k €]" totalsRowFunction="custom" dataDxfId="116" totalsRowDxfId="20">
+    <tableColumn id="4" name="3 [k €]" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="25">
       <calculatedColumnFormula>IF(F69=$M$70,$M$70,$E$92/(F69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[3]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4 [k €]" totalsRowFunction="custom" dataDxfId="115" totalsRowDxfId="19">
+    <tableColumn id="5" name="4 [k €]" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="23">
       <calculatedColumnFormula>IF(G69=$M$70,$M$70,$E$92/(G69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[4]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5 [k €]" totalsRowFunction="custom" dataDxfId="114" totalsRowDxfId="18">
+    <tableColumn id="6" name="5 [k €]" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="21">
       <calculatedColumnFormula>IF(H69=$M$70,$M$70,$E$92/(H69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[5]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6 [k €]" totalsRowFunction="custom" dataDxfId="113" totalsRowDxfId="17">
+    <tableColumn id="7" name="6 [k €]" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="19">
       <calculatedColumnFormula>IF(I69=$M$70,$M$70,$E$92/(I69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[6]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7 [k €]" totalsRowFunction="custom" dataDxfId="112" totalsRowDxfId="16">
+    <tableColumn id="8" name="7 [k €]" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="17">
       <calculatedColumnFormula>IF(J69=$M$70,$M$70,$E$92/(J69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[7]]*1000)</totalsRowFormula>
     </tableColumn>
@@ -42954,20 +42962,20 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B56</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="111">
+    <tableColumn id="2" name="CPI" dataDxfId="10">
       <calculatedColumnFormula>Kennzahlen!J69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="110">
+    <tableColumn id="3" name="SPI" dataDxfId="9">
       <calculatedColumnFormula>Kennzahlen!J82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="109">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="8">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="108"/>
-    <tableColumn id="6" name="Status" dataDxfId="107">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="7"/>
+    <tableColumn id="6" name="Status" dataDxfId="6">
       <calculatedColumnFormula>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Trend" dataDxfId="106">
+    <tableColumn id="7" name="Trend" dataDxfId="5">
       <calculatedColumnFormula>IF(C18=Kennzahlen!$M$70,Kennzahlen!$M$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -42982,19 +42990,19 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="105">
+    <tableColumn id="2" name="CPI" dataDxfId="4">
       <calculatedColumnFormula>Kennzahlen!I69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="104">
+    <tableColumn id="3" name="SPI" dataDxfId="3">
       <calculatedColumnFormula>Kennzahlen!I82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="103">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="2">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="102">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="1">
       <calculatedColumnFormula>F5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Status" dataDxfId="101">
+    <tableColumn id="6" name="Status" dataDxfId="0">
       <calculatedColumnFormula>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Trend"/>
@@ -43016,36 +43024,36 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="144">
+    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="137">
       <calculatedColumnFormula>B17</calculatedColumnFormula>
       <totalsRowFormula>AC[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="9" name="0" totalsRowLabel="0"/>
-    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="143" totalsRowDxfId="57">
+    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="136" totalsRowDxfId="135">
       <calculatedColumnFormula>D4*'Fertigstellungsgrad der Akt.'!B2</calculatedColumnFormula>
       <totalsRowFormula>SUM(EV[1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="142" totalsRowDxfId="56">
+    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="134" totalsRowDxfId="133">
       <calculatedColumnFormula>E4*'Fertigstellungsgrad der Akt.'!C2</calculatedColumnFormula>
       <totalsRowFormula>SUM(EV[2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="141" totalsRowDxfId="55">
+    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="132" totalsRowDxfId="131">
       <calculatedColumnFormula>F4*'Fertigstellungsgrad der Akt.'!D2</calculatedColumnFormula>
       <totalsRowFormula>SUM(EV[3])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="140" totalsRowDxfId="54">
+    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="130" totalsRowDxfId="129">
       <calculatedColumnFormula>G4*'Fertigstellungsgrad der Akt.'!E2</calculatedColumnFormula>
       <totalsRowFormula>SUM(EV[4])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="139" totalsRowDxfId="53">
+    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="128" totalsRowDxfId="127">
       <calculatedColumnFormula>H4*'Fertigstellungsgrad der Akt.'!F2</calculatedColumnFormula>
       <totalsRowFormula>SUM(EV[5])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="138" totalsRowDxfId="52">
+    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="126" totalsRowDxfId="125">
       <calculatedColumnFormula>I4*'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
       <totalsRowFormula>SUM(EV[6])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="137" totalsRowDxfId="51">
+    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="124" totalsRowDxfId="123">
       <calculatedColumnFormula>J4*'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
       <totalsRowFormula>SUM(EV[7])</totalsRowFormula>
     </tableColumn>
@@ -43067,31 +43075,31 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="136">
+    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="122">
       <calculatedColumnFormula>B4</calculatedColumnFormula>
       <totalsRowFormula>PV[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
     <tableColumn id="9" name="0" totalsRowLabel="0"/>
-    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="135" totalsRowDxfId="71">
+    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="121" totalsRowDxfId="120">
       <calculatedColumnFormula>'Tatsächliche Kosten'!B2*'Tatsächliche Kosten'!$B$15</calculatedColumnFormula>
       <totalsRowFormula>SUM('Tatsächliche Kosten'!$B12:'Tatsächliche Kosten'!B12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="134" totalsRowDxfId="70">
+    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="119" totalsRowDxfId="118">
       <totalsRowFormula>SUM('Tatsächliche Kosten'!$B12:'Tatsächliche Kosten'!C12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="133" totalsRowDxfId="69">
+    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="117" totalsRowDxfId="116">
       <totalsRowFormula>SUM('Tatsächliche Kosten'!$B12:'Tatsächliche Kosten'!D12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="132" totalsRowDxfId="68">
+    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="115" totalsRowDxfId="114">
       <totalsRowFormula>SUM('Tatsächliche Kosten'!$B12:'Tatsächliche Kosten'!E12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="131" totalsRowDxfId="67">
+    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="113" totalsRowDxfId="112">
       <totalsRowFormula>SUM('Tatsächliche Kosten'!$B12:'Tatsächliche Kosten'!F12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="130" totalsRowDxfId="66">
+    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="111" totalsRowDxfId="110">
       <totalsRowFormula>SUM('Tatsächliche Kosten'!$B12:'Tatsächliche Kosten'!G12)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="129" totalsRowDxfId="65">
+    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="109" totalsRowDxfId="108">
       <totalsRowFormula>SUM('Tatsächliche Kosten'!$B12:'Tatsächliche Kosten'!H12)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -43116,35 +43124,35 @@
       <calculatedColumnFormula>B30</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" name="0" totalsRowFunction="custom" totalsRowDxfId="87">
+    <tableColumn id="9" name="0" totalsRowFunction="custom" totalsRowDxfId="107">
       <calculatedColumnFormula>C30-C17</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[0]]-AC[[#Totals],[0]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="100" totalsRowDxfId="86">
+    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="106" totalsRowDxfId="105">
       <calculatedColumnFormula>D30-D17</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[1]]-AC[[#Totals],[1]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="99" totalsRowDxfId="85">
+    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="104" totalsRowDxfId="103">
       <calculatedColumnFormula>E30-E17</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[2]]-AC[[#Totals],[2]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="98" totalsRowDxfId="84">
+    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="102" totalsRowDxfId="101">
       <calculatedColumnFormula>F30-F17</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[3]]-AC[[#Totals],[3]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="97" totalsRowDxfId="83">
+    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="100" totalsRowDxfId="99">
       <calculatedColumnFormula>G30-G17</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[4]]-AC[[#Totals],[4]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="96" totalsRowDxfId="82">
+    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="98" totalsRowDxfId="97">
       <calculatedColumnFormula>H30-H17</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[5]]-AC[[#Totals],[5]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="95" totalsRowDxfId="81">
+    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="96" totalsRowDxfId="95">
       <calculatedColumnFormula>I30-I17</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[6]]-AC[[#Totals],[6]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="94" totalsRowDxfId="80">
+    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="94" totalsRowDxfId="93">
       <calculatedColumnFormula>J30-J17</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[7]]-AC[[#Totals],[7]]</totalsRowFormula>
     </tableColumn>
@@ -43161,35 +43169,35 @@
       <calculatedColumnFormula>B43</calculatedColumnFormula>
       <totalsRowFormula>CV[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" name="0" totalsRowFunction="custom" totalsRowDxfId="79">
+    <tableColumn id="9" name="0" totalsRowFunction="custom" totalsRowDxfId="92">
       <calculatedColumnFormula>C30-C4</calculatedColumnFormula>
       <totalsRowFormula>SUM(SV[0])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="128" totalsRowDxfId="78">
+    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="91" totalsRowDxfId="90">
       <calculatedColumnFormula>D30-D4</calculatedColumnFormula>
       <totalsRowFormula>SUM(SV[1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="127" totalsRowDxfId="77">
+    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="89" totalsRowDxfId="88">
       <calculatedColumnFormula>E30-E4</calculatedColumnFormula>
       <totalsRowFormula>SUM(SV[2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="126" totalsRowDxfId="76">
+    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="87" totalsRowDxfId="86">
       <calculatedColumnFormula>F30-F4</calculatedColumnFormula>
       <totalsRowFormula>SUM(SV[3])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="125" totalsRowDxfId="75">
+    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="85" totalsRowDxfId="84">
       <calculatedColumnFormula>G30-G4</calculatedColumnFormula>
       <totalsRowFormula>SUM(SV[4])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="124" totalsRowDxfId="74">
+    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="83" totalsRowDxfId="82">
       <calculatedColumnFormula>H30-H4</calculatedColumnFormula>
       <totalsRowFormula>SUM(SV[5])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="123" totalsRowDxfId="73">
+    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="81" totalsRowDxfId="80">
       <calculatedColumnFormula>I30-I4</calculatedColumnFormula>
       <totalsRowFormula>SUM(SV[6])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="122" totalsRowDxfId="72">
+    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="79" totalsRowDxfId="78">
       <calculatedColumnFormula>J30-J4</calculatedColumnFormula>
       <totalsRowFormula>SUM(SV[7])</totalsRowFormula>
     </tableColumn>
@@ -43206,34 +43214,34 @@
       <calculatedColumnFormula>B56</calculatedColumnFormula>
       <totalsRowFormula>SV[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" name="0" totalsRowFunction="custom" totalsRowDxfId="15">
+    <tableColumn id="9" name="0" totalsRowFunction="custom" totalsRowDxfId="77">
       <totalsRowFormula>1</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="14">
+    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="76" totalsRowDxfId="75">
       <calculatedColumnFormula>IF(D17=0,$M$83,D30/D17)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[1]]/AC[[#Totals],[1]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="44" totalsRowDxfId="13">
+    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="74" totalsRowDxfId="73">
       <calculatedColumnFormula>IF(E17=0,$M$83,E30/E17)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[2]]/AC[[#Totals],[2]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="12">
+    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="72" totalsRowDxfId="71">
       <calculatedColumnFormula>IF(F17=0,$M$83,F30/F17)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[3]]/AC[[#Totals],[3]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="11">
+    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="70" totalsRowDxfId="69">
       <calculatedColumnFormula>IF(G17=0,$M$83,G30/G17)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[4]]/AC[[#Totals],[4]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="10">
+    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="68" totalsRowDxfId="67">
       <calculatedColumnFormula>IF(H17=0,$M$83,H30/H17)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[5]]/AC[[#Totals],[5]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="9">
+    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="66" totalsRowDxfId="65">
       <calculatedColumnFormula>IF(I17=0,$M$83,I30/I17)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[6]]/AC[[#Totals],[6]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="121" totalsRowDxfId="8">
+    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="64" totalsRowDxfId="63">
       <calculatedColumnFormula>IF(J17=0,"-",J30/J17)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[7]]/AC[[#Totals],[7]]</totalsRowFormula>
     </tableColumn>
@@ -43250,34 +43258,34 @@
       <calculatedColumnFormula>B69</calculatedColumnFormula>
       <totalsRowFormula>CPI[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" name="0" totalsRowFunction="custom" totalsRowDxfId="7">
+    <tableColumn id="9" name="0" totalsRowFunction="custom" totalsRowDxfId="62">
       <totalsRowFormula>1</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="50" totalsRowDxfId="6">
+    <tableColumn id="2" name="1" totalsRowFunction="custom" dataDxfId="61" totalsRowDxfId="60">
       <calculatedColumnFormula>IF(D4=0,$M$83,D30/D4)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[1]]/PV[[#Totals],[1]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="5">
+    <tableColumn id="3" name="2" totalsRowFunction="custom" dataDxfId="59" totalsRowDxfId="58">
       <calculatedColumnFormula>IF(E4=0,$M$83,E30/E4)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[2]]/PV[[#Totals],[2]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="48" totalsRowDxfId="4">
+    <tableColumn id="4" name="3" totalsRowFunction="custom" dataDxfId="57" totalsRowDxfId="56">
       <calculatedColumnFormula>IF(F4=0,$M$83,F30/F4)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[3]]/PV[[#Totals],[3]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="3">
+    <tableColumn id="5" name="4" totalsRowFunction="custom" dataDxfId="55" totalsRowDxfId="54">
       <calculatedColumnFormula>IF(G4=0,$M$83,G30/G4)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[4]]/PV[[#Totals],[4]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="2">
+    <tableColumn id="6" name="5" totalsRowFunction="custom" dataDxfId="53" totalsRowDxfId="52">
       <calculatedColumnFormula>IF(H4=0,$M$83,H30/H4)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[5]]/PV[[#Totals],[5]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="1">
+    <tableColumn id="7" name="6" totalsRowFunction="custom" dataDxfId="51" totalsRowDxfId="50">
       <calculatedColumnFormula>IF(I4=0,$M$83,I30/I4)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[6]]/PV[[#Totals],[6]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="120" totalsRowDxfId="0">
+    <tableColumn id="8" name="7" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="48">
       <calculatedColumnFormula>IF(J4=0,"-",J30/J4)</calculatedColumnFormula>
       <totalsRowFormula>EV[[#Totals],[7]]/PV[[#Totals],[7]]</totalsRowFormula>
     </tableColumn>
@@ -43307,39 +43315,39 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="ETC" displayName="ETC" ref="B96:J104" totalsRowCount="1">
   <autoFilter ref="B96:J103"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="38">
+    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="47">
       <calculatedColumnFormula>B82</calculatedColumnFormula>
       <totalsRowFormula>SPI[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" name="0 [k €]" totalsRowFunction="custom" dataDxfId="23">
+    <tableColumn id="9" name="0 [k €]" totalsRowFunction="custom" dataDxfId="46">
       <calculatedColumnFormula>'Budgetierte Kosten'!P2/1000</calculatedColumnFormula>
       <totalsRowFormula>'Budgetierte Kosten'!P11/1000</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="1 [k €]" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="30">
+    <tableColumn id="2" name="1 [k €]" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="44">
       <calculatedColumnFormula>IF(D69=$M$70,$M$70,('Budgetierte Kosten'!$P2-D30)/(D69*1000))</calculatedColumnFormula>
       <totalsRowFormula>($E$92-EV[[#Totals],[1]])/(CPI[[#Totals],[1]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2 [k €]" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="29">
+    <tableColumn id="3" name="2 [k €]" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="42">
       <calculatedColumnFormula>IF(E69=$M$70,$M$70,($E$92-E30)/(E69*1000))</calculatedColumnFormula>
       <totalsRowFormula>($E$92-EV[[#Totals],[2]])/(CPI[[#Totals],[2]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3 [k €]" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="28">
+    <tableColumn id="4" name="3 [k €]" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="40">
       <calculatedColumnFormula>IF(F69=$M$70,$M$70,($E$92-F30)/(F69*1000))</calculatedColumnFormula>
       <totalsRowFormula>($E$92-EV[[#Totals],[3]])/(CPI[[#Totals],[3]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4 [k €]" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="27">
+    <tableColumn id="5" name="4 [k €]" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="38">
       <calculatedColumnFormula>IF(G69=$M$70,$M$70,($E$92-G30)/(G69*1000))</calculatedColumnFormula>
       <totalsRowFormula>($E$92-EV[[#Totals],[4]])/(CPI[[#Totals],[4]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5 [k €]" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="26">
+    <tableColumn id="6" name="5 [k €]" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="36">
       <calculatedColumnFormula>IF(H69=$M$70,$M$70,($E$92-H30)/(H69*1000))</calculatedColumnFormula>
       <totalsRowFormula>($E$92-EV[[#Totals],[5]])/(CPI[[#Totals],[5]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6 [k €]" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="25">
+    <tableColumn id="7" name="6 [k €]" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="34">
       <calculatedColumnFormula>IF(I69=$M$70,$M$70,($E$92-I30)/(I69*1000))</calculatedColumnFormula>
       <totalsRowFormula>($E$92-EV[[#Totals],[6]])/(CPI[[#Totals],[6]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7 [k €]" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="24">
+    <tableColumn id="8" name="7 [k €]" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="32">
       <calculatedColumnFormula>IF(J69=$M$70,$M$70,($E$92-J30)/(J69*1000))</calculatedColumnFormula>
       <totalsRowFormula>($E$92-EV[[#Totals],[7]])/(CPI[[#Totals],[7]]*1000)</totalsRowFormula>
     </tableColumn>
@@ -43732,23 +43740,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y124"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L87" sqref="L87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="23.25">
       <c r="A1" s="27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -43807,7 +43815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25">
       <c r="B4" t="str">
         <f>'Budgetierte Kosten'!A2</f>
         <v>Anforderungsanalyse</v>
@@ -43844,7 +43852,7 @@
         <v>144000</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25">
       <c r="B5" t="str">
         <f>'Budgetierte Kosten'!A3</f>
         <v>Design und Architektur</v>
@@ -43881,7 +43889,7 @@
         <v>172000</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25">
       <c r="B6" t="str">
         <f>'Budgetierte Kosten'!A4</f>
         <v>Implementierung</v>
@@ -43918,7 +43926,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25">
       <c r="B7" t="str">
         <f>'Budgetierte Kosten'!A5</f>
         <v>Integration und Test</v>
@@ -43955,7 +43963,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25">
       <c r="B8" t="str">
         <f>'Budgetierte Kosten'!A6</f>
         <v>Projektmanagement</v>
@@ -43992,7 +44000,7 @@
         <v>154000</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25">
       <c r="B9" t="str">
         <f>'Budgetierte Kosten'!A7</f>
         <v>Puffer für unerwartetes</v>
@@ -44029,7 +44037,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -44071,7 +44079,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25">
       <c r="B11" t="s">
         <v>80</v>
       </c>
@@ -44107,7 +44115,7 @@
         <v>723000</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25">
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
@@ -44116,7 +44124,7 @@
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25">
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
@@ -44132,12 +44140,12 @@
         <v>723000</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="23.25">
       <c r="A14" s="27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -44166,7 +44174,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="B17" t="str">
         <f t="shared" ref="B17:B23" si="0">B4</f>
         <v>Anforderungsanalyse</v>
@@ -44209,7 +44217,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>Design und Architektur</v>
@@ -44246,7 +44254,7 @@
         <v>87550</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v>Implementierung</v>
@@ -44283,7 +44291,7 @@
         <v>42500</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v>Integration und Test</v>
@@ -44320,7 +44328,7 @@
         <v>29750</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v>Projektmanagement</v>
@@ -44357,7 +44365,7 @@
         <v>204000</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v>Puffer für unerwartetes</v>
@@ -44394,7 +44402,7 @@
         <v>353600</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>Materialkosten</v>
@@ -44431,7 +44439,7 @@
         <v>16200</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="B24" t="str">
         <f>PV[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -44475,7 +44483,7 @@
         <v>83600</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="L25" s="2" t="s">
         <v>89</v>
       </c>
@@ -44484,12 +44492,12 @@
         <v>868750</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="23.25">
       <c r="A27" s="27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="B29" t="s">
         <v>16</v>
       </c>
@@ -44518,7 +44526,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="str">
         <f t="shared" ref="B30:B36" si="1">B17</f>
         <v>Anforderungsanalyse</v>
@@ -44561,7 +44569,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="B31" t="str">
         <f t="shared" si="1"/>
         <v>Design und Architektur</v>
@@ -44598,7 +44606,7 @@
         <v>94400</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="B32" t="str">
         <f t="shared" si="1"/>
         <v>Implementierung</v>
@@ -44635,7 +44643,7 @@
         <v>98000</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22">
       <c r="B33" t="str">
         <f t="shared" si="1"/>
         <v>Integration und Test</v>
@@ -44672,7 +44680,7 @@
         <v>63000</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22">
       <c r="B34" t="str">
         <f t="shared" si="1"/>
         <v>Projektmanagement</v>
@@ -44709,7 +44717,7 @@
         <v>143000</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22">
       <c r="B35" t="str">
         <f t="shared" si="1"/>
         <v>Puffer für unerwartetes</v>
@@ -44746,7 +44754,7 @@
         <v>57200.000000000007</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22">
       <c r="B36" t="str">
         <f t="shared" si="1"/>
         <v>Materialkosten</v>
@@ -44783,7 +44791,7 @@
         <v>12040.000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22">
       <c r="B37" t="str">
         <f>AC[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -44820,7 +44828,7 @@
         <v>597240</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:22" ht="23.25">
       <c r="A40" s="27" t="s">
         <v>32</v>
       </c>
@@ -44828,7 +44836,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22">
       <c r="B42" t="s">
         <v>16</v>
       </c>
@@ -44881,41 +44889,41 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22">
       <c r="B43" t="str">
         <f t="shared" ref="B43:B49" si="2">B30</f>
         <v>Anforderungsanalyse</v>
       </c>
       <c r="C43" s="28">
-        <f>C30-C17</f>
+        <f t="shared" ref="C43:J43" si="3">C30-C17</f>
         <v>0</v>
       </c>
       <c r="D43" s="28">
-        <f>D30-D17</f>
+        <f t="shared" si="3"/>
         <v>7900</v>
       </c>
       <c r="E43" s="28">
-        <f>E30-E17</f>
+        <f t="shared" si="3"/>
         <v>-77800</v>
       </c>
       <c r="F43" s="28">
-        <f>F30-F17</f>
+        <f t="shared" si="3"/>
         <v>-116500</v>
       </c>
       <c r="G43" s="28">
-        <f>G30-G17</f>
+        <f t="shared" si="3"/>
         <v>-91950</v>
       </c>
       <c r="H43" s="28">
-        <f>H30-H17</f>
+        <f t="shared" si="3"/>
         <v>-63150</v>
       </c>
       <c r="I43" s="28">
-        <f>I30-I17</f>
+        <f t="shared" si="3"/>
         <v>-19950</v>
       </c>
       <c r="J43" s="28">
-        <f>J30-J17</f>
+        <f t="shared" si="3"/>
         <v>-5550</v>
       </c>
       <c r="L43" s="2" t="s">
@@ -44949,235 +44957,235 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22">
       <c r="B44" t="str">
         <f t="shared" si="2"/>
         <v>Design und Architektur</v>
       </c>
       <c r="C44" s="28">
-        <f t="shared" ref="C44:C49" si="3">C31-C18</f>
+        <f t="shared" ref="C44:C49" si="4">C31-C18</f>
         <v>0</v>
       </c>
       <c r="D44" s="28">
-        <f>D31-D18</f>
+        <f t="shared" ref="D44:J49" si="5">D31-D18</f>
         <v>0</v>
       </c>
       <c r="E44" s="28">
-        <f>E31-E18</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F44" s="28">
-        <f>F31-F18</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G44" s="28">
-        <f>G31-G18</f>
+        <f t="shared" si="5"/>
         <v>-30700</v>
       </c>
       <c r="H44" s="28">
-        <f>H31-H18</f>
+        <f t="shared" si="5"/>
         <v>-47700</v>
       </c>
       <c r="I44" s="28">
-        <f>I31-I18</f>
+        <f t="shared" si="5"/>
         <v>-55450</v>
       </c>
       <c r="J44" s="28">
-        <f>J31-J18</f>
+        <f t="shared" si="5"/>
         <v>6850</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22">
       <c r="B45" t="str">
         <f t="shared" si="2"/>
         <v>Implementierung</v>
       </c>
       <c r="C45" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D45" s="28">
-        <f>D32-D19</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E45" s="28">
-        <f>E32-E19</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F45" s="28">
-        <f>F32-F19</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G45" s="28">
-        <f>G32-G19</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H45" s="28">
-        <f>H32-H19</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I45" s="28">
-        <f>I32-I19</f>
+        <f t="shared" si="5"/>
         <v>17950</v>
       </c>
       <c r="J45" s="28">
-        <f>J32-J19</f>
+        <f t="shared" si="5"/>
         <v>55500</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22">
       <c r="B46" t="str">
         <f t="shared" si="2"/>
         <v>Integration und Test</v>
       </c>
       <c r="C46" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D46" s="28">
-        <f>D33-D20</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E46" s="28">
-        <f>E33-E20</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F46" s="28">
-        <f>F33-F20</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G46" s="28">
-        <f>G33-G20</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H46" s="28">
-        <f>H33-H20</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I46" s="28">
-        <f>I33-I20</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J46" s="28">
-        <f>J33-J20</f>
+        <f t="shared" si="5"/>
         <v>33250</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22">
       <c r="B47" t="str">
         <f t="shared" si="2"/>
         <v>Projektmanagement</v>
       </c>
       <c r="C47" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D47" s="28">
-        <f>D34-D21</f>
+        <f t="shared" si="5"/>
         <v>-2620</v>
       </c>
       <c r="E47" s="28">
-        <f>E34-E21</f>
+        <f t="shared" si="5"/>
         <v>-79200</v>
       </c>
       <c r="F47" s="28">
-        <f>F34-F21</f>
+        <f t="shared" si="5"/>
         <v>-84600</v>
       </c>
       <c r="G47" s="28">
-        <f>G34-G21</f>
+        <f t="shared" si="5"/>
         <v>-95800</v>
       </c>
       <c r="H47" s="28">
-        <f>H34-H21</f>
+        <f t="shared" si="5"/>
         <v>-84200</v>
       </c>
       <c r="I47" s="28">
-        <f>I34-I21</f>
+        <f t="shared" si="5"/>
         <v>-72600</v>
       </c>
       <c r="J47" s="28">
-        <f>J34-J21</f>
+        <f t="shared" si="5"/>
         <v>-61000</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22">
       <c r="B48" t="str">
         <f t="shared" si="2"/>
         <v>Puffer für unerwartetes</v>
       </c>
       <c r="C48" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D48" s="28">
-        <f>D35-D22</f>
+        <f t="shared" si="5"/>
         <v>-5280</v>
       </c>
       <c r="E48" s="28">
-        <f>E35-E22</f>
+        <f t="shared" si="5"/>
         <v>-161400</v>
       </c>
       <c r="F48" s="28">
-        <f>F35-F22</f>
+        <f t="shared" si="5"/>
         <v>-292200</v>
       </c>
       <c r="G48" s="28">
-        <f>G35-G22</f>
+        <f t="shared" si="5"/>
         <v>-320050</v>
       </c>
       <c r="H48" s="28">
-        <f>H35-H22</f>
+        <f t="shared" si="5"/>
         <v>-313900</v>
       </c>
       <c r="I48" s="28">
-        <f>I35-I22</f>
+        <f t="shared" si="5"/>
         <v>-302550</v>
       </c>
       <c r="J48" s="28">
-        <f>J35-J22</f>
+        <f t="shared" si="5"/>
         <v>-296400</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13">
       <c r="B49" t="str">
         <f t="shared" si="2"/>
         <v>Materialkosten</v>
       </c>
       <c r="C49" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D49" s="28">
-        <f>D36-D23</f>
+        <f t="shared" si="5"/>
         <v>-280</v>
       </c>
       <c r="E49" s="28">
-        <f>E36-E23</f>
+        <f t="shared" si="5"/>
         <v>-60</v>
       </c>
       <c r="F49" s="28">
-        <f>F36-F23</f>
+        <f t="shared" si="5"/>
         <v>260</v>
       </c>
       <c r="G49" s="28">
-        <f>G36-G23</f>
+        <f t="shared" si="5"/>
         <v>480</v>
       </c>
       <c r="H49" s="28">
-        <f>H36-H23</f>
+        <f t="shared" si="5"/>
         <v>1200</v>
       </c>
       <c r="I49" s="28">
-        <f>I36-I23</f>
+        <f t="shared" si="5"/>
         <v>-4680</v>
       </c>
       <c r="J49" s="28">
-        <f>J36-J23</f>
+        <f t="shared" si="5"/>
         <v>-4159.9999999999982</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13">
       <c r="B50" t="str">
         <f>EV[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -45222,7 +45230,7 @@
         <v>-280</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13">
       <c r="L51" s="2" t="s">
         <v>89</v>
       </c>
@@ -45231,12 +45239,12 @@
         <v>-271510</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" ht="23.25">
       <c r="A53" s="27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13">
       <c r="B55" t="s">
         <v>16</v>
       </c>
@@ -45265,41 +45273,41 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13">
       <c r="B56" t="str">
-        <f t="shared" ref="B56:B62" si="4">B43</f>
+        <f t="shared" ref="B56:B62" si="6">B43</f>
         <v>Anforderungsanalyse</v>
       </c>
       <c r="C56" s="28">
-        <f>C30-C4</f>
+        <f t="shared" ref="C56:J56" si="7">C30-C4</f>
         <v>0</v>
       </c>
       <c r="D56" s="28">
-        <f>D30-D4</f>
+        <f t="shared" si="7"/>
         <v>2400</v>
       </c>
       <c r="E56" s="28">
-        <f>E30-E4</f>
+        <f t="shared" si="7"/>
         <v>-88800</v>
       </c>
       <c r="F56" s="28">
-        <f>F30-F4</f>
+        <f t="shared" si="7"/>
         <v>-129600</v>
       </c>
       <c r="G56" s="28">
-        <f>G30-G4</f>
+        <f t="shared" si="7"/>
         <v>-100800</v>
       </c>
       <c r="H56" s="28">
-        <f>H30-H4</f>
+        <f t="shared" si="7"/>
         <v>-72000</v>
       </c>
       <c r="I56" s="28">
-        <f>I30-I4</f>
+        <f t="shared" si="7"/>
         <v>-28800</v>
       </c>
       <c r="J56" s="28">
-        <f>J30-J4</f>
+        <f t="shared" si="7"/>
         <v>-14400</v>
       </c>
       <c r="L56" s="2" t="s">
@@ -45309,231 +45317,231 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13">
       <c r="B57" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Design und Architektur</v>
       </c>
       <c r="C57" s="28">
-        <f t="shared" ref="C57:C62" si="5">C31-C5</f>
+        <f t="shared" ref="C57:C62" si="8">C31-C5</f>
         <v>0</v>
       </c>
       <c r="D57" s="28">
-        <f>D31-D5</f>
+        <f t="shared" ref="D57:J62" si="9">D31-D5</f>
         <v>0</v>
       </c>
       <c r="E57" s="28">
-        <f>E31-E5</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F57" s="28">
-        <f>F31-F5</f>
+        <f t="shared" si="9"/>
         <v>-20000</v>
       </c>
       <c r="G57" s="28">
-        <f>G31-G5</f>
+        <f t="shared" si="9"/>
         <v>-40200</v>
       </c>
       <c r="H57" s="28">
-        <f>H31-H5</f>
+        <f t="shared" si="9"/>
         <v>-84200</v>
       </c>
       <c r="I57" s="28">
-        <f>I31-I5</f>
+        <f t="shared" si="9"/>
         <v>-128400</v>
       </c>
       <c r="J57" s="28">
-        <f>J31-J5</f>
+        <f t="shared" si="9"/>
         <v>-77600</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13">
       <c r="B58" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Implementierung</v>
       </c>
       <c r="C58" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D58" s="28">
-        <f>D32-D6</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E58" s="28">
-        <f>E32-E6</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F58" s="28">
-        <f>F32-F6</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G58" s="28">
-        <f>G32-G6</f>
+        <f t="shared" si="9"/>
         <v>-24000</v>
       </c>
       <c r="H58" s="28">
-        <f>H32-H6</f>
+        <f t="shared" si="9"/>
         <v>-64000</v>
       </c>
       <c r="I58" s="28">
-        <f>I32-I6</f>
+        <f t="shared" si="9"/>
         <v>-72800</v>
       </c>
       <c r="J58" s="28">
-        <f>J32-J6</f>
+        <f t="shared" si="9"/>
         <v>-62000</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13">
       <c r="B59" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Integration und Test</v>
       </c>
       <c r="C59" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D59" s="28">
-        <f>D33-D7</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E59" s="28">
-        <f>E33-E7</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F59" s="28">
-        <f>F33-F7</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G59" s="28">
-        <f>G33-G7</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H59" s="28">
-        <f>H33-H7</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I59" s="28">
-        <f>I33-I7</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J59" s="28">
-        <f>J33-J7</f>
+        <f t="shared" si="9"/>
         <v>47000</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13">
       <c r="B60" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Projektmanagement</v>
       </c>
       <c r="C60" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D60" s="28">
-        <f>D34-D8</f>
+        <f t="shared" si="9"/>
         <v>880</v>
       </c>
       <c r="E60" s="28">
-        <f>E34-E8</f>
+        <f t="shared" si="9"/>
         <v>-29700</v>
       </c>
       <c r="F60" s="28">
-        <f>F34-F8</f>
+        <f t="shared" si="9"/>
         <v>-23100</v>
       </c>
       <c r="G60" s="28">
-        <f>G34-G8</f>
+        <f t="shared" si="9"/>
         <v>-30800</v>
       </c>
       <c r="H60" s="28">
-        <f>H34-H8</f>
+        <f t="shared" si="9"/>
         <v>-24200</v>
       </c>
       <c r="I60" s="28">
-        <f>I34-I8</f>
+        <f t="shared" si="9"/>
         <v>-17600</v>
       </c>
       <c r="J60" s="28">
-        <f>J34-J8</f>
+        <f t="shared" si="9"/>
         <v>-11000</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13">
       <c r="B61" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Puffer für unerwartetes</v>
       </c>
       <c r="C61" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D61" s="28">
-        <f>D35-D9</f>
+        <f t="shared" si="9"/>
         <v>320</v>
       </c>
       <c r="E61" s="28">
-        <f>E35-E9</f>
+        <f t="shared" si="9"/>
         <v>-10800</v>
       </c>
       <c r="F61" s="28">
-        <f>F35-F9</f>
+        <f t="shared" si="9"/>
         <v>-13600</v>
       </c>
       <c r="G61" s="28">
-        <f>G35-G9</f>
+        <f t="shared" si="9"/>
         <v>-11200</v>
       </c>
       <c r="H61" s="28">
-        <f>H35-H9</f>
+        <f t="shared" si="9"/>
         <v>-8800</v>
       </c>
       <c r="I61" s="28">
-        <f>I35-I9</f>
+        <f t="shared" si="9"/>
         <v>-1200</v>
       </c>
       <c r="J61" s="28">
-        <f>J35-J9</f>
+        <f t="shared" si="9"/>
         <v>1200.0000000000073</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13">
       <c r="B62" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Materialkosten</v>
       </c>
       <c r="C62" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D62" s="28">
-        <f>D36-D10</f>
+        <f t="shared" si="9"/>
         <v>-280</v>
       </c>
       <c r="E62" s="28">
-        <f>E36-E10</f>
+        <f t="shared" si="9"/>
         <v>-560</v>
       </c>
       <c r="F62" s="28">
-        <f>F36-F10</f>
+        <f t="shared" si="9"/>
         <v>-1840</v>
       </c>
       <c r="G62" s="28">
-        <f>G36-G10</f>
+        <f t="shared" si="9"/>
         <v>-3120</v>
       </c>
       <c r="H62" s="28">
-        <f>H36-H10</f>
+        <f t="shared" si="9"/>
         <v>-4400</v>
       </c>
       <c r="I62" s="28">
-        <f>I36-I10</f>
+        <f t="shared" si="9"/>
         <v>-5680</v>
       </c>
       <c r="J62" s="28">
-        <f>J36-J10</f>
+        <f t="shared" si="9"/>
         <v>-8959.9999999999982</v>
       </c>
       <c r="L62" s="2" t="s">
@@ -45544,7 +45552,7 @@
         <v>3320</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13">
       <c r="B63" t="str">
         <f>CV[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -45589,7 +45597,7 @@
         <v>-125760</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:22" ht="23.25">
       <c r="A66" s="27" t="s">
         <v>34</v>
       </c>
@@ -45597,7 +45605,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:22">
       <c r="B68" t="s">
         <v>16</v>
       </c>
@@ -45650,40 +45658,40 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:22">
       <c r="B69" t="str">
-        <f t="shared" ref="B69:B75" si="6">B56</f>
+        <f t="shared" ref="B69:B75" si="10">B56</f>
         <v>Anforderungsanalyse</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69" s="29">
-        <f t="shared" ref="D69:D75" si="7">IF(D17=0,$M$83,D30/D17)</f>
+        <f t="shared" ref="D69:D75" si="11">IF(D17=0,$M$83,D30/D17)</f>
         <v>1.1858823529411764</v>
       </c>
       <c r="E69" s="29">
-        <f t="shared" ref="E69:E75" si="8">IF(E17=0,$M$83,E30/E17)</f>
+        <f t="shared" ref="E69:E75" si="12">IF(E17=0,$M$83,E30/E17)</f>
         <v>8.4705882352941173E-2</v>
       </c>
       <c r="F69" s="29">
-        <f t="shared" ref="F69:F75" si="9">IF(F17=0,$M$83,F30/F17)</f>
+        <f t="shared" ref="F69:F75" si="13">IF(F17=0,$M$83,F30/F17)</f>
         <v>0.11000763941940413</v>
       </c>
       <c r="G69" s="29">
-        <f t="shared" ref="G69:G75" si="10">IF(G17=0,$M$83,G30/G17)</f>
+        <f t="shared" ref="G69:G75" si="14">IF(G17=0,$M$83,G30/G17)</f>
         <v>0.31964483906770258</v>
       </c>
       <c r="H69" s="29">
-        <f t="shared" ref="H69:H75" si="11">IF(H17=0,$M$83,H30/H17)</f>
+        <f t="shared" ref="H69:H75" si="15">IF(H17=0,$M$83,H30/H17)</f>
         <v>0.53274139844617097</v>
       </c>
       <c r="I69" s="29">
-        <f t="shared" ref="I69:I75" si="12">IF(I17=0,$M$83,I30/I17)</f>
+        <f t="shared" ref="I69:I75" si="16">IF(I17=0,$M$83,I30/I17)</f>
         <v>0.85238623751387343</v>
       </c>
       <c r="J69" s="29">
-        <f>IF(J17=0,"-",J30/J17)</f>
+        <f t="shared" ref="J69:J75" si="17">IF(J17=0,"-",J30/J17)</f>
         <v>0.95893451720310763</v>
       </c>
       <c r="L69" s="2" t="s">
@@ -45720,9 +45728,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:22">
       <c r="B70" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>Design und Architektur</v>
       </c>
       <c r="C70">
@@ -45730,31 +45738,31 @@
         <v>1</v>
       </c>
       <c r="D70" s="29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E70" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="F70" s="29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="G70" s="29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0.27764705882352941</v>
       </c>
       <c r="H70" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0.19831932773109243</v>
       </c>
       <c r="I70" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.29854522454142945</v>
       </c>
       <c r="J70" s="29">
-        <f>IF(J18=0,"-",J31/J18)</f>
+        <f t="shared" si="17"/>
         <v>1.0782410051399201</v>
       </c>
       <c r="L70" t="s">
@@ -45764,9 +45772,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:22">
       <c r="B71" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>Implementierung</v>
       </c>
       <c r="C71">
@@ -45774,37 +45782,37 @@
         <v>1</v>
       </c>
       <c r="D71" s="29">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E71" s="29">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="F71" s="29">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="G71" s="29">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="H71" s="29">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
+      <c r="E71" s="29">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="F71" s="29">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="G71" s="29">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="H71" s="29">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
       <c r="I71" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.8447058823529412</v>
       </c>
       <c r="J71" s="29">
-        <f>IF(J19=0,"-",J32/J19)</f>
+        <f t="shared" si="17"/>
         <v>2.3058823529411763</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22">
       <c r="B72" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>Integration und Test</v>
       </c>
       <c r="C72">
@@ -45812,146 +45820,146 @@
         <v>1</v>
       </c>
       <c r="D72" s="29">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E72" s="29">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="F72" s="29">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="G72" s="29">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="H72" s="29">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="I72" s="29">
+      <c r="E72" s="29">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
+      <c r="F72" s="29">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="G72" s="29">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="H72" s="29">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="I72" s="29">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
       <c r="J72" s="29">
-        <f>IF(J20=0,"-",J33/J20)</f>
+        <f t="shared" si="17"/>
         <v>2.1176470588235294</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:22">
       <c r="B73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>Projektmanagement</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73" s="29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.89725490196078428</v>
       </c>
       <c r="E73" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.15294117647058825</v>
       </c>
       <c r="F73" s="29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.33647058823529413</v>
       </c>
       <c r="G73" s="29">
+        <f t="shared" si="14"/>
+        <v>0.3738562091503268</v>
+      </c>
+      <c r="H73" s="29">
+        <f t="shared" si="15"/>
+        <v>0.50470588235294123</v>
+      </c>
+      <c r="I73" s="29">
+        <f t="shared" si="16"/>
+        <v>0.61176470588235299</v>
+      </c>
+      <c r="J73" s="29">
+        <f t="shared" si="17"/>
+        <v>0.7009803921568627</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22">
+      <c r="B74" t="str">
         <f t="shared" si="10"/>
-        <v>0.3738562091503268</v>
-      </c>
-      <c r="H73" s="29">
-        <f t="shared" si="11"/>
-        <v>0.50470588235294123</v>
-      </c>
-      <c r="I73" s="29">
-        <f t="shared" si="12"/>
-        <v>0.61176470588235299</v>
-      </c>
-      <c r="J73" s="29">
-        <f>IF(J21=0,"-",J34/J21)</f>
-        <v>0.7009803921568627</v>
-      </c>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B74" t="str">
-        <f t="shared" si="6"/>
         <v>Puffer für unerwartetes</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74" s="29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.61176470588235299</v>
       </c>
       <c r="E74" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3.1212484993997598E-2</v>
       </c>
       <c r="F74" s="29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>3.4368803701255786E-2</v>
       </c>
       <c r="G74" s="29">
+        <f t="shared" si="14"/>
+        <v>6.1023910811207276E-2</v>
+      </c>
+      <c r="H74" s="29">
+        <f t="shared" si="15"/>
+        <v>9.040857722399305E-2</v>
+      </c>
+      <c r="I74" s="29">
+        <f t="shared" si="16"/>
+        <v>0.13396307428080723</v>
+      </c>
+      <c r="J74" s="29">
+        <f t="shared" si="17"/>
+        <v>0.16176470588235295</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22">
+      <c r="B75" t="str">
         <f t="shared" si="10"/>
-        <v>6.1023910811207276E-2</v>
-      </c>
-      <c r="H74" s="29">
-        <f t="shared" si="11"/>
-        <v>9.040857722399305E-2</v>
-      </c>
-      <c r="I74" s="29">
-        <f t="shared" si="12"/>
-        <v>0.13396307428080723</v>
-      </c>
-      <c r="J74" s="29">
-        <f>IF(J22=0,"-",J35/J22)</f>
-        <v>0.16176470588235295</v>
-      </c>
-    </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B75" t="str">
-        <f t="shared" si="6"/>
         <v>Materialkosten</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" s="29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.86</v>
       </c>
       <c r="E75" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.98285714285714287</v>
       </c>
       <c r="F75" s="29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.0530612244897959</v>
       </c>
       <c r="G75" s="29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1.075</v>
       </c>
       <c r="H75" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1.1621621621621621</v>
       </c>
       <c r="I75" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.68799999999999994</v>
       </c>
       <c r="J75" s="29">
-        <f>IF(J23=0,"-",J36/J23)</f>
+        <f t="shared" si="17"/>
         <v>0.74320987654321002</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:22">
       <c r="B76" t="str">
         <f>SV[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -45989,12 +45997,12 @@
         <v>0.68747050359712225</v>
       </c>
     </row>
-    <row r="79" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:22" ht="23.25">
       <c r="A79" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18">
       <c r="B81" t="s">
         <v>16</v>
       </c>
@@ -46023,40 +46031,40 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18">
       <c r="B82" t="str">
-        <f t="shared" ref="B82:B88" si="13">B69</f>
+        <f t="shared" ref="B82:B88" si="18">B69</f>
         <v>Anforderungsanalyse</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82" s="29">
-        <f t="shared" ref="D82:D88" si="14">IF(D4=0,$M$83,D30/D4)</f>
+        <f t="shared" ref="D82:D88" si="19">IF(D4=0,$M$83,D30/D4)</f>
         <v>1.05</v>
       </c>
       <c r="E82" s="29">
-        <f t="shared" ref="E82:E88" si="15">IF(E4=0,$M$83,E30/E4)</f>
+        <f t="shared" ref="E82:E88" si="20">IF(E4=0,$M$83,E30/E4)</f>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="F82" s="29">
-        <f t="shared" ref="F82:F88" si="16">IF(F4=0,$M$83,F30/F4)</f>
+        <f t="shared" ref="F82:F88" si="21">IF(F4=0,$M$83,F30/F4)</f>
         <v>0.1</v>
       </c>
       <c r="G82" s="29">
-        <f t="shared" ref="G82:G88" si="17">IF(G4=0,$M$83,G30/G4)</f>
+        <f t="shared" ref="G82:G88" si="22">IF(G4=0,$M$83,G30/G4)</f>
         <v>0.3</v>
       </c>
       <c r="H82" s="29">
-        <f t="shared" ref="H82:H88" si="18">IF(H4=0,$M$83,H30/H4)</f>
+        <f t="shared" ref="H82:H88" si="23">IF(H4=0,$M$83,H30/H4)</f>
         <v>0.5</v>
       </c>
       <c r="I82" s="29">
-        <f t="shared" ref="I82:I88" si="19">IF(I4=0,$M$83,I30/I4)</f>
+        <f t="shared" ref="I82:I88" si="24">IF(I4=0,$M$83,I30/I4)</f>
         <v>0.8</v>
       </c>
       <c r="J82" s="29">
-        <f>IF(J4=0,"-",J30/J4)</f>
+        <f t="shared" ref="J82:J88" si="25">IF(J4=0,"-",J30/J4)</f>
         <v>0.9</v>
       </c>
       <c r="L82" s="2" t="s">
@@ -46069,9 +46077,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18">
       <c r="B83" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>Design und Architektur</v>
       </c>
       <c r="C83">
@@ -46079,31 +46087,31 @@
         <v>1</v>
       </c>
       <c r="D83" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="E83" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="F83" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="G83" s="29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>0.22692307692307692</v>
       </c>
       <c r="H83" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0.12291666666666666</v>
       </c>
       <c r="I83" s="29">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.15526315789473685</v>
       </c>
       <c r="J83" s="29">
-        <f>IF(J5=0,"-",J31/J5)</f>
+        <f t="shared" si="25"/>
         <v>0.5488372093023256</v>
       </c>
       <c r="L83" t="s">
@@ -46113,9 +46121,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18">
       <c r="B84" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>Implementierung</v>
       </c>
       <c r="C84">
@@ -46123,37 +46131,37 @@
         <v>1</v>
       </c>
       <c r="D84" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="E84" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="F84" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="G84" s="29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H84" s="29">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="I84" s="29">
+        <f t="shared" si="24"/>
+        <v>0.35</v>
+      </c>
+      <c r="J84" s="29">
+        <f t="shared" si="25"/>
+        <v>0.61250000000000004</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18">
+      <c r="B85" t="str">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="I84" s="29">
-        <f t="shared" si="19"/>
-        <v>0.35</v>
-      </c>
-      <c r="J84" s="29">
-        <f>IF(J6=0,"-",J32/J6)</f>
-        <v>0.61250000000000004</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B85" t="str">
-        <f t="shared" si="13"/>
         <v>Integration und Test</v>
       </c>
       <c r="C85">
@@ -46161,146 +46169,146 @@
         <v>1</v>
       </c>
       <c r="D85" s="29">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="E85" s="29">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="F85" s="29">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="G85" s="29">
-        <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-      <c r="H85" s="29">
-        <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="I85" s="29">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
+      <c r="E85" s="29">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="F85" s="29">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="G85" s="29">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="H85" s="29">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="I85" s="29">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
       <c r="J85" s="29">
-        <f>IF(J7=0,"-",J33/J7)</f>
+        <f t="shared" si="25"/>
         <v>3.9375</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18">
       <c r="B86" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>Projektmanagement</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
       <c r="D86" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.04</v>
       </c>
       <c r="E86" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0.32500000000000001</v>
       </c>
       <c r="F86" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.65</v>
       </c>
       <c r="G86" s="29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>0.65</v>
       </c>
       <c r="H86" s="29">
+        <f t="shared" si="23"/>
+        <v>0.78</v>
+      </c>
+      <c r="I86" s="29">
+        <f t="shared" si="24"/>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="J86" s="29">
+        <f t="shared" si="25"/>
+        <v>0.9285714285714286</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="B87" t="str">
         <f t="shared" si="18"/>
-        <v>0.78</v>
-      </c>
-      <c r="I86" s="29">
-        <f t="shared" si="19"/>
-        <v>0.8666666666666667</v>
-      </c>
-      <c r="J86" s="29">
-        <f>IF(J8=0,"-",J34/J8)</f>
-        <v>0.9285714285714286</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B87" t="str">
-        <f t="shared" si="13"/>
         <v>Puffer für unerwartetes</v>
       </c>
       <c r="C87">
         <v>1</v>
       </c>
       <c r="D87" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.04</v>
       </c>
       <c r="E87" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0.32500000000000001</v>
       </c>
       <c r="F87" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.43333333333333335</v>
       </c>
       <c r="G87" s="29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>0.65</v>
       </c>
       <c r="H87" s="29">
+        <f t="shared" si="23"/>
+        <v>0.78</v>
+      </c>
+      <c r="I87" s="29">
+        <f t="shared" si="24"/>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J87" s="29">
+        <f t="shared" si="25"/>
+        <v>1.0214285714285716</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18">
+      <c r="B88" t="str">
         <f t="shared" si="18"/>
-        <v>0.78</v>
-      </c>
-      <c r="I87" s="29">
-        <f t="shared" si="19"/>
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="J87" s="29">
-        <f>IF(J9=0,"-",J35/J9)</f>
-        <v>1.0214285714285716</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B88" t="str">
-        <f t="shared" si="13"/>
         <v>Materialkosten</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
       <c r="D88" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>0.86</v>
       </c>
       <c r="E88" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0.86</v>
       </c>
       <c r="F88" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.7371428571428571</v>
       </c>
       <c r="G88" s="29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>0.68799999999999994</v>
       </c>
       <c r="H88" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0.66153846153846152</v>
       </c>
       <c r="I88" s="29">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.64500000000000002</v>
       </c>
       <c r="J88" s="29">
-        <f>IF(J10=0,"-",J36/J10)</f>
+        <f t="shared" si="25"/>
         <v>0.57333333333333347</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18">
       <c r="B89" t="str">
         <f>CPI[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -46338,7 +46346,7 @@
         <v>0.82605809128630703</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:18" ht="23.25">
       <c r="A92" s="33" t="s">
         <v>69</v>
       </c>
@@ -46346,17 +46354,17 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:18" ht="23.25">
       <c r="A94" s="27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:18">
       <c r="N95" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:18">
       <c r="B96" t="s">
         <v>16</v>
       </c>
@@ -46397,9 +46405,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:18">
       <c r="B97" t="str">
-        <f t="shared" ref="B97:B103" si="20">B82</f>
+        <f t="shared" ref="B97:B103" si="26">B82</f>
         <v>Anforderungsanalyse</v>
       </c>
       <c r="C97">
@@ -46449,7 +46457,7 @@
         <v>144000</v>
       </c>
       <c r="Q97" s="28">
-        <f>J30</f>
+        <f t="shared" ref="Q97:Q103" si="27">J30</f>
         <v>129600</v>
       </c>
       <c r="R97" s="28">
@@ -46457,9 +46465,9 @@
         <v>14400</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18">
       <c r="B98" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>Design und Architektur</v>
       </c>
       <c r="C98">
@@ -46503,17 +46511,17 @@
         <v>236000</v>
       </c>
       <c r="Q98" s="28">
-        <f>J31</f>
+        <f t="shared" si="27"/>
         <v>94400</v>
       </c>
       <c r="R98" s="28">
-        <f t="shared" ref="R98:R103" si="21">P98-Q98</f>
+        <f t="shared" ref="R98:R103" si="28">P98-Q98</f>
         <v>141600</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18">
       <c r="B99" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>Implementierung</v>
       </c>
       <c r="C99">
@@ -46557,17 +46565,17 @@
         <v>392000</v>
       </c>
       <c r="Q99" s="28">
-        <f>J32</f>
+        <f t="shared" si="27"/>
         <v>98000</v>
       </c>
       <c r="R99" s="28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>294000</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:18">
       <c r="B100" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>Integration und Test</v>
       </c>
       <c r="C100">
@@ -46611,17 +46619,17 @@
         <v>252000</v>
       </c>
       <c r="Q100" s="28">
-        <f>J33</f>
+        <f t="shared" si="27"/>
         <v>63000</v>
       </c>
       <c r="R100" s="28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>189000</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18">
       <c r="B101" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>Projektmanagement</v>
       </c>
       <c r="C101">
@@ -46665,17 +46673,17 @@
         <v>286000</v>
       </c>
       <c r="Q101" s="28">
-        <f>J34</f>
+        <f t="shared" si="27"/>
         <v>143000</v>
       </c>
       <c r="R101" s="28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>143000</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18">
       <c r="B102" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>Puffer für unerwartetes</v>
       </c>
       <c r="C102">
@@ -46719,17 +46727,17 @@
         <v>104000</v>
       </c>
       <c r="Q102" s="28">
-        <f>J35</f>
+        <f t="shared" si="27"/>
         <v>57200.000000000007</v>
       </c>
       <c r="R102" s="28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>46799.999999999993</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:18">
       <c r="B103" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>Materialkosten</v>
       </c>
       <c r="C103">
@@ -46773,15 +46781,15 @@
         <v>86000</v>
       </c>
       <c r="Q103" s="28">
-        <f>J36</f>
+        <f t="shared" si="27"/>
         <v>12040.000000000002</v>
       </c>
       <c r="R103" s="28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>73960</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:18">
       <c r="B104" t="str">
         <f>SPI[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -46819,7 +46827,7 @@
         <v>1313.1617942535665</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18">
       <c r="K106" s="2" t="s">
         <v>89</v>
       </c>
@@ -46828,12 +46836,12 @@
         <v>955.91504329004329</v>
       </c>
     </row>
-    <row r="107" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:18" ht="23.25">
       <c r="A107" s="33" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18">
       <c r="B109" t="s">
         <v>16</v>
       </c>
@@ -46862,9 +46870,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18">
       <c r="B110" t="str">
-        <f t="shared" ref="B110:C116" si="22">B97</f>
+        <f t="shared" ref="B110:C116" si="29">B97</f>
         <v>Anforderungsanalyse</v>
       </c>
       <c r="C110">
@@ -46906,13 +46914,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:18">
       <c r="B111" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>Design und Architektur</v>
       </c>
       <c r="C111">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>236</v>
       </c>
       <c r="D111" s="29">
@@ -46944,13 +46952,13 @@
         <v>218.87499999999997</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18">
       <c r="B112" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>Implementierung</v>
       </c>
       <c r="C112">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>392</v>
       </c>
       <c r="D112" s="29">
@@ -46982,13 +46990,13 @@
         <v>170.00000000000003</v>
       </c>
     </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:13">
       <c r="B113" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>Integration und Test</v>
       </c>
       <c r="C113">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>252</v>
       </c>
       <c r="D113" s="29">
@@ -47020,13 +47028,13 @@
         <v>119.00000000000001</v>
       </c>
     </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:13">
       <c r="B114" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>Projektmanagement</v>
       </c>
       <c r="C114">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>286</v>
       </c>
       <c r="D114" s="29">
@@ -47058,13 +47066,13 @@
         <v>408.00000000000006</v>
       </c>
     </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:13">
       <c r="B115" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>Puffer für unerwartetes</v>
       </c>
       <c r="C115">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>104</v>
       </c>
       <c r="D115" s="29">
@@ -47096,13 +47104,13 @@
         <v>642.90909090909088</v>
       </c>
     </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:13">
       <c r="B116" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>Materialkosten</v>
       </c>
       <c r="C116">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>86</v>
       </c>
       <c r="D116" s="29">
@@ -47134,7 +47142,7 @@
         <v>115.71428571428569</v>
       </c>
     </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:13">
       <c r="B117" t="str">
         <f>ETC[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -47179,45 +47187,45 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:13">
       <c r="L118">
-        <f>J111*J70</f>
+        <f t="shared" ref="L118:L124" si="30">J111*J70</f>
         <v>235.99999999999997</v>
       </c>
     </row>
-    <row r="119" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:13">
       <c r="L119">
-        <f>J112*J71</f>
+        <f t="shared" si="30"/>
         <v>392.00000000000006</v>
       </c>
     </row>
-    <row r="120" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:13">
       <c r="L120">
-        <f>J113*J72</f>
+        <f t="shared" si="30"/>
         <v>252.00000000000003</v>
       </c>
     </row>
-    <row r="121" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:13">
       <c r="L121">
-        <f>J114*J73</f>
+        <f t="shared" si="30"/>
         <v>286</v>
       </c>
     </row>
-    <row r="122" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:13">
       <c r="L122">
-        <f>J115*J74</f>
+        <f t="shared" si="30"/>
         <v>104</v>
       </c>
     </row>
-    <row r="123" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:13">
       <c r="L123">
-        <f>J116*J75</f>
+        <f t="shared" si="30"/>
         <v>86</v>
       </c>
     </row>
-    <row r="124" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:13">
       <c r="L124">
-        <f>J117*J76</f>
+        <f t="shared" si="30"/>
         <v>1499.9999999999998</v>
       </c>
       <c r="M124">
@@ -47252,7 +47260,7 @@
       <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
@@ -47261,12 +47269,12 @@
     <col min="10" max="10" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="23.25">
       <c r="A2" s="27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="J3" t="s">
         <v>48</v>
       </c>
@@ -47274,7 +47282,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -47303,7 +47311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="B5" t="str">
         <f>Kennzahlen!B56</f>
         <v>Anforderungsanalyse</v>
@@ -47333,7 +47341,7 @@
         <v>POS</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="B6" t="str">
         <f>Kennzahlen!B57</f>
         <v>Design und Architektur</v>
@@ -47369,7 +47377,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="B7" t="str">
         <f>Kennzahlen!B58</f>
         <v>Implementierung</v>
@@ -47405,7 +47413,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="B8" t="str">
         <f>Kennzahlen!B59</f>
         <v>Integration und Test</v>
@@ -47441,7 +47449,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="B9" t="str">
         <f>Kennzahlen!B60</f>
         <v>Projektmanagement</v>
@@ -47471,7 +47479,7 @@
         <v>POS</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="B10" t="str">
         <f>Kennzahlen!B61</f>
         <v>Puffer für unerwartetes</v>
@@ -47507,7 +47515,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="B11" t="str">
         <f>Kennzahlen!B62</f>
         <v>Materialkosten</v>
@@ -47543,7 +47551,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="B12" t="str">
         <f>Kennzahlen!B63</f>
         <v>Gesamt</v>
@@ -47578,7 +47586,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="J13" t="s">
         <v>66</v>
       </c>
@@ -47586,12 +47594,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="23.25">
       <c r="A15" s="27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -47614,7 +47622,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8">
       <c r="B18" t="str">
         <f>Kennzahlen!B69</f>
         <v>Anforderungsanalyse</v>
@@ -47640,7 +47648,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8">
       <c r="B19" t="str">
         <f>Kennzahlen!B70</f>
         <v>Design und Architektur</v>
@@ -47666,7 +47674,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8">
       <c r="B20" t="str">
         <f>Kennzahlen!B71</f>
         <v>Implementierung</v>
@@ -47692,7 +47700,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8">
       <c r="B21" t="str">
         <f>Kennzahlen!B72</f>
         <v>Integration und Test</v>
@@ -47718,7 +47726,7 @@
         <v>Grün</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8">
       <c r="B22" t="str">
         <f>Kennzahlen!B73</f>
         <v>Projektmanagement</v>
@@ -47744,7 +47752,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8">
       <c r="B23" t="str">
         <f>Kennzahlen!B74</f>
         <v>Puffer für unerwartetes</v>
@@ -47770,7 +47778,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8">
       <c r="B24" t="str">
         <f>Kennzahlen!B75</f>
         <v>Materialkosten</v>
@@ -47796,7 +47804,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8">
       <c r="B25" t="str">
         <f>Kennzahlen!B76</f>
         <v>Gesamt</v>
@@ -47824,13 +47832,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:D12 C18:D25">
-    <cfRule type="cellIs" dxfId="93" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="greaterThanOrEqual">
       <formula>$K$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="lessThan">
       <formula>$K$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
       <formula>$K$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47889,11 +47897,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I151" sqref="I151"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="R33" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -47909,7 +47917,7 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
@@ -47924,7 +47932,7 @@
     <col min="16" max="16" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="12.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -47975,7 +47983,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="12.95" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -48031,7 +48039,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="12.95" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -48087,7 +48095,7 @@
         <v>0.15733333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="12.95" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -48143,7 +48151,7 @@
         <v>0.26133333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="12.95" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -48199,7 +48207,7 @@
         <v>0.16800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="12.95" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -48255,7 +48263,7 @@
         <v>0.19066666666666668</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="12.95" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -48311,7 +48319,7 @@
         <v>6.933333333333333E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" s="2" customFormat="1" ht="12.95" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -48376,11 +48384,11 @@
         <v>1414000</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="12.95" customHeight="1">
       <c r="A9" s="9"/>
       <c r="P9" s="10"/>
     </row>
-    <row r="10" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="12.95" customHeight="1">
       <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
@@ -48441,7 +48449,7 @@
       </c>
       <c r="P10" s="10"/>
     </row>
-    <row r="11" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="12.95" customHeight="1">
       <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
@@ -48497,7 +48505,7 @@
         <v>5.7333333333333333E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" s="2" customFormat="1" ht="12.95" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -48555,7 +48563,7 @@
       </c>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="12.95" customHeight="1">
       <c r="A13" s="15"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -48570,7 +48578,7 @@
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
     </row>
-    <row r="14" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="12.95" customHeight="1">
       <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
@@ -48593,12 +48601,12 @@
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
     </row>
-    <row r="17" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="12.95" customHeight="1">
       <c r="A17" s="36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="12.95" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -48644,7 +48652,7 @@
       <c r="O18" s="2"/>
       <c r="P18" s="3"/>
     </row>
-    <row r="19" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="12.95" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>1</v>
       </c>
@@ -48703,7 +48711,7 @@
       <c r="O19" s="6"/>
       <c r="P19" s="7"/>
     </row>
-    <row r="20" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="12.95" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>2</v>
       </c>
@@ -48762,7 +48770,7 @@
       <c r="O20" s="6"/>
       <c r="P20" s="7"/>
     </row>
-    <row r="21" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="12.95" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>3</v>
       </c>
@@ -48821,7 +48829,7 @@
       <c r="O21" s="6"/>
       <c r="P21" s="7"/>
     </row>
-    <row r="22" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="12.95" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
@@ -48880,7 +48888,7 @@
       <c r="O22" s="6"/>
       <c r="P22" s="7"/>
     </row>
-    <row r="23" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="12.95" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -48939,7 +48947,7 @@
       <c r="O23" s="6"/>
       <c r="P23" s="7"/>
     </row>
-    <row r="24" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="12.95" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>6</v>
       </c>
@@ -48998,7 +49006,7 @@
       <c r="O24" s="6"/>
       <c r="P24" s="7"/>
     </row>
-    <row r="25" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="12.95" customHeight="1">
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
@@ -49057,7 +49065,7 @@
       <c r="O25" s="2"/>
       <c r="P25" s="8"/>
     </row>
-    <row r="26" spans="1:16" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" s="2" customFormat="1" ht="12.95" customHeight="1">
       <c r="A26" s="37" t="s">
         <v>80</v>
       </c>
@@ -49130,7 +49138,7 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="8" width="9.42578125" customWidth="1"/>
@@ -49142,7 +49150,7 @@
     <col min="16" max="16" width="12.28515625" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="12.95" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -49174,7 +49182,7 @@
       <c r="O1" s="22"/>
       <c r="P1" s="23"/>
     </row>
-    <row r="2" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="12.95" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
@@ -49200,7 +49208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="12.95" customHeight="1">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
@@ -49226,7 +49234,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="12.95" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
@@ -49252,7 +49260,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="12.95" customHeight="1">
       <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
@@ -49278,7 +49286,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="12.95" customHeight="1">
       <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
@@ -49304,7 +49312,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="12.95" customHeight="1">
       <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
@@ -49330,7 +49338,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="12.95" customHeight="1">
       <c r="A8" s="2" t="str">
         <f>'Budgetierte Kosten'!A8</f>
         <v>Summe Personenstunden pro Monat</v>
@@ -49364,7 +49372,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="12.95" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -49374,7 +49382,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="12.95" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -49407,7 +49415,7 @@
         <v>80750</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="12.95" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -49441,7 +49449,7 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
     </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" s="2" customFormat="1" ht="12.95" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -49482,7 +49490,7 @@
       <c r="O12" s="24"/>
       <c r="P12" s="25"/>
     </row>
-    <row r="15" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="12.95" customHeight="1">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -49506,7 +49514,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="3" width="10.140625" customWidth="1"/>
@@ -49515,7 +49523,7 @@
     <col min="12" max="13" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="12.95" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -49546,7 +49554,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="12.95" customHeight="1">
       <c r="A2" s="15" t="str">
         <f>'Budgetierte Kosten'!A2</f>
         <v>Anforderungsanalyse</v>
@@ -49573,7 +49581,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="12.95" customHeight="1">
       <c r="A3" s="15" t="str">
         <f>'Budgetierte Kosten'!A3</f>
         <v>Design und Architektur</v>
@@ -49600,7 +49608,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="12.95" customHeight="1">
       <c r="A4" s="15" t="str">
         <f>'Budgetierte Kosten'!A4</f>
         <v>Implementierung</v>
@@ -49627,7 +49635,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="12.95" customHeight="1">
       <c r="A5" s="15" t="str">
         <f>'Budgetierte Kosten'!A5</f>
         <v>Integration und Test</v>
@@ -49654,7 +49662,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="12.95" customHeight="1">
       <c r="A6" s="15" t="str">
         <f>'Budgetierte Kosten'!A6</f>
         <v>Projektmanagement</v>
@@ -49681,7 +49689,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="12.95" customHeight="1">
       <c r="A7" s="15" t="str">
         <f>'Budgetierte Kosten'!A7</f>
         <v>Puffer für unerwartetes</v>
@@ -49708,7 +49716,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="12.95" customHeight="1">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -49739,7 +49747,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="12.95" customHeight="1">
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
@@ -49753,7 +49761,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="12.95" customHeight="1">
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
@@ -49767,12 +49775,12 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="12.95" customHeight="1">
       <c r="A11" s="38" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="12.95" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -49798,7 +49806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="12.95" customHeight="1">
       <c r="A13" s="15" t="str">
         <f>'Budgetierte Kosten'!A2</f>
         <v>Anforderungsanalyse</v>
@@ -49832,7 +49840,7 @@
         <v>8.6400000000000005E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="12.95" customHeight="1">
       <c r="A14" s="15" t="str">
         <f>'Budgetierte Kosten'!A3</f>
         <v>Design und Architektur</v>
@@ -49866,7 +49874,7 @@
         <v>6.2933333333333327E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="12.95" customHeight="1">
       <c r="A15" s="15" t="str">
         <f>'Budgetierte Kosten'!A4</f>
         <v>Implementierung</v>
@@ -49900,7 +49908,7 @@
         <v>6.5333333333333327E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="12.95" customHeight="1">
       <c r="A16" s="15" t="str">
         <f>'Budgetierte Kosten'!A5</f>
         <v>Integration und Test</v>
@@ -49934,7 +49942,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="12.95" customHeight="1">
       <c r="A17" s="15" t="str">
         <f>'Budgetierte Kosten'!A6</f>
         <v>Projektmanagement</v>
@@ -49968,7 +49976,7 @@
         <v>9.5333333333333339E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="12.95" customHeight="1">
       <c r="A18" s="15" t="str">
         <f>'Budgetierte Kosten'!A7</f>
         <v>Puffer für unerwartetes</v>
@@ -50002,7 +50010,7 @@
         <v>3.8133333333333332E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="12.95" customHeight="1">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -50035,7 +50043,7 @@
         <v>8.0266666666666681E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="12.95" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Potenzielle Entscheidungen + Anmerkungen überarbeitet
</commit_message>
<xml_diff>
--- a/Lab1/Auswertung Final.xlsx
+++ b/Lab1/Auswertung Final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sack\Christian\A\Studium\4 - Semester\SpBC\Übungen\swpbc\Lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SK\Dropbox\033 534 - Bachelorstudium Software &amp; Information Engineering\__LVAs\Softwareprojekt-Beobachtung und -Controlling\UE1\GIT repo\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -314,7 +314,7 @@
     <numFmt numFmtId="168" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1336,7 +1336,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1756,7 +1756,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1794,7 +1794,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -1856,7 +1856,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -1908,7 +1908,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1938,7 +1938,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2000,7 +2000,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2412,7 +2412,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2450,7 +2450,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -2512,7 +2512,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -2564,7 +2564,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2594,7 +2594,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2656,7 +2656,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3068,7 +3068,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3106,7 +3106,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -3168,7 +3168,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -3220,7 +3220,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3250,7 +3250,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3312,7 +3312,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3724,7 +3724,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3762,7 +3762,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -3824,7 +3824,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -3876,7 +3876,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3906,7 +3906,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3968,7 +3968,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4380,7 +4380,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4418,7 +4418,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -4480,7 +4480,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -4532,7 +4532,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4562,7 +4562,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4624,7 +4624,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5036,7 +5036,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5074,7 +5074,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -5136,7 +5136,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -5188,7 +5188,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5218,7 +5218,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5280,7 +5280,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5601,7 +5601,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5639,7 +5639,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -5719,7 +5719,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5757,7 +5757,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -5809,7 +5809,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5839,7 +5839,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5901,7 +5901,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6222,7 +6222,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6260,7 +6260,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -6340,7 +6340,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6378,7 +6378,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -6430,7 +6430,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6460,7 +6460,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6522,7 +6522,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6843,7 +6843,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6881,7 +6881,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -6961,7 +6961,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6999,7 +6999,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -7051,7 +7051,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7081,7 +7081,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7143,7 +7143,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7464,7 +7464,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7502,7 +7502,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -7582,7 +7582,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7620,7 +7620,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -7672,7 +7672,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7702,7 +7702,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7764,7 +7764,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8085,7 +8085,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8123,7 +8123,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -8203,7 +8203,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8241,7 +8241,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -8293,7 +8293,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -8323,7 +8323,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8385,7 +8385,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8805,7 +8805,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8843,7 +8843,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -8905,7 +8905,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -8957,7 +8957,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -8987,7 +8987,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9049,7 +9049,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9370,7 +9370,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9408,7 +9408,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -9488,7 +9488,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9526,7 +9526,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -9578,7 +9578,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9608,7 +9608,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9670,7 +9670,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9991,7 +9991,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10029,7 +10029,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -10109,7 +10109,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10147,7 +10147,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -10199,7 +10199,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -10229,7 +10229,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10291,7 +10291,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -10711,7 +10711,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10749,7 +10749,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -10811,7 +10811,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -10863,7 +10863,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -10893,7 +10893,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10955,7 +10955,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -11367,7 +11367,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11405,7 +11405,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -11467,7 +11467,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -11519,7 +11519,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11549,7 +11549,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11611,7 +11611,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -11932,7 +11932,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11970,7 +11970,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -12050,7 +12050,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12088,7 +12088,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -12140,7 +12140,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -12170,7 +12170,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -12246,7 +12246,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -12966,7 +12966,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -13003,7 +13003,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="363062264"/>
@@ -13093,7 +13093,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -13125,7 +13125,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="363063576"/>
@@ -13180,7 +13180,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -13210,7 +13210,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -13272,7 +13272,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -13700,7 +13700,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -13738,7 +13738,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -13800,7 +13800,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -13852,7 +13852,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -13882,7 +13882,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -13944,7 +13944,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -14372,7 +14372,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -14410,7 +14410,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -14472,7 +14472,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -14524,7 +14524,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -14554,7 +14554,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -14616,7 +14616,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -15044,7 +15044,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -15082,7 +15082,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -15144,7 +15144,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -15196,7 +15196,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -15226,7 +15226,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -15288,7 +15288,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -15740,7 +15740,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -15778,7 +15778,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -15840,7 +15840,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -15892,7 +15892,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -15922,7 +15922,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -15984,7 +15984,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -16404,7 +16404,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -16442,7 +16442,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -16504,7 +16504,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -16556,7 +16556,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -16586,7 +16586,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -16648,7 +16648,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -17076,7 +17076,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -17114,7 +17114,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -17176,7 +17176,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -17228,7 +17228,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -17258,7 +17258,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -17320,7 +17320,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -17748,7 +17748,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -17786,7 +17786,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -17848,7 +17848,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -17900,7 +17900,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -17930,7 +17930,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -17992,7 +17992,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -18420,7 +18420,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -18458,7 +18458,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -18520,7 +18520,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -18572,7 +18572,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -18602,7 +18602,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -18664,7 +18664,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -19092,7 +19092,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -19130,7 +19130,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -19192,7 +19192,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -19244,7 +19244,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -19274,7 +19274,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -19336,7 +19336,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -19756,7 +19756,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -19794,7 +19794,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -19856,7 +19856,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -19908,7 +19908,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -19938,7 +19938,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -20000,7 +20000,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -20420,7 +20420,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -20458,7 +20458,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -20520,7 +20520,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -20572,7 +20572,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -20602,7 +20602,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -20664,7 +20664,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -21084,7 +21084,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -21122,7 +21122,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -21184,7 +21184,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -21236,7 +21236,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -21266,7 +21266,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -21328,7 +21328,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -21748,7 +21748,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -21786,7 +21786,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -21848,7 +21848,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -21900,7 +21900,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -21930,7 +21930,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -21992,7 +21992,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -22404,7 +22404,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -22442,7 +22442,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -22504,7 +22504,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -22556,7 +22556,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -22586,7 +22586,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -22648,7 +22648,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -23060,7 +23060,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -23098,7 +23098,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270221696"/>
@@ -23160,7 +23160,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270223336"/>
@@ -23212,7 +23212,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -23242,7 +23242,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -43740,23 +43740,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y124"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L87" sqref="L87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="23.25">
+    <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -43815,7 +43815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B4" t="str">
         <f>'Budgetierte Kosten'!A2</f>
         <v>Anforderungsanalyse</v>
@@ -43852,7 +43852,7 @@
         <v>144000</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B5" t="str">
         <f>'Budgetierte Kosten'!A3</f>
         <v>Design und Architektur</v>
@@ -43889,7 +43889,7 @@
         <v>172000</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B6" t="str">
         <f>'Budgetierte Kosten'!A4</f>
         <v>Implementierung</v>
@@ -43926,7 +43926,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B7" t="str">
         <f>'Budgetierte Kosten'!A5</f>
         <v>Integration und Test</v>
@@ -43963,7 +43963,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B8" t="str">
         <f>'Budgetierte Kosten'!A6</f>
         <v>Projektmanagement</v>
@@ -44000,7 +44000,7 @@
         <v>154000</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B9" t="str">
         <f>'Budgetierte Kosten'!A7</f>
         <v>Puffer für unerwartetes</v>
@@ -44037,7 +44037,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -44079,7 +44079,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>80</v>
       </c>
@@ -44115,7 +44115,7 @@
         <v>723000</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
@@ -44124,7 +44124,7 @@
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
@@ -44140,12 +44140,12 @@
         <v>723000</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="23.25">
+    <row r="14" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -44174,7 +44174,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B17" t="str">
         <f t="shared" ref="B17:B23" si="0">B4</f>
         <v>Anforderungsanalyse</v>
@@ -44217,7 +44217,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>Design und Architektur</v>
@@ -44254,7 +44254,7 @@
         <v>87550</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v>Implementierung</v>
@@ -44291,7 +44291,7 @@
         <v>42500</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v>Integration und Test</v>
@@ -44328,7 +44328,7 @@
         <v>29750</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v>Projektmanagement</v>
@@ -44365,7 +44365,7 @@
         <v>204000</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v>Puffer für unerwartetes</v>
@@ -44402,7 +44402,7 @@
         <v>353600</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>Materialkosten</v>
@@ -44439,7 +44439,7 @@
         <v>16200</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" t="str">
         <f>PV[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -44483,7 +44483,7 @@
         <v>83600</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L25" s="2" t="s">
         <v>89</v>
       </c>
@@ -44492,12 +44492,12 @@
         <v>868750</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="23.25">
+    <row r="27" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A27" s="27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>16</v>
       </c>
@@ -44526,7 +44526,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" t="str">
         <f t="shared" ref="B30:B36" si="1">B17</f>
         <v>Anforderungsanalyse</v>
@@ -44569,7 +44569,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" t="str">
         <f t="shared" si="1"/>
         <v>Design und Architektur</v>
@@ -44606,7 +44606,7 @@
         <v>94400</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" t="str">
         <f t="shared" si="1"/>
         <v>Implementierung</v>
@@ -44643,7 +44643,7 @@
         <v>98000</v>
       </c>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B33" t="str">
         <f t="shared" si="1"/>
         <v>Integration und Test</v>
@@ -44680,7 +44680,7 @@
         <v>63000</v>
       </c>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B34" t="str">
         <f t="shared" si="1"/>
         <v>Projektmanagement</v>
@@ -44717,7 +44717,7 @@
         <v>143000</v>
       </c>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B35" t="str">
         <f t="shared" si="1"/>
         <v>Puffer für unerwartetes</v>
@@ -44754,7 +44754,7 @@
         <v>57200.000000000007</v>
       </c>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B36" t="str">
         <f t="shared" si="1"/>
         <v>Materialkosten</v>
@@ -44791,7 +44791,7 @@
         <v>12040.000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B37" t="str">
         <f>AC[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -44828,7 +44828,7 @@
         <v>597240</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="23.25">
+    <row r="40" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A40" s="27" t="s">
         <v>32</v>
       </c>
@@ -44836,7 +44836,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:22">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>16</v>
       </c>
@@ -44889,7 +44889,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:22">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B43" t="str">
         <f t="shared" ref="B43:B49" si="2">B30</f>
         <v>Anforderungsanalyse</v>
@@ -44957,7 +44957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:22">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B44" t="str">
         <f t="shared" si="2"/>
         <v>Design und Architektur</v>
@@ -44995,7 +44995,7 @@
         <v>6850</v>
       </c>
     </row>
-    <row r="45" spans="1:22">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B45" t="str">
         <f t="shared" si="2"/>
         <v>Implementierung</v>
@@ -45033,7 +45033,7 @@
         <v>55500</v>
       </c>
     </row>
-    <row r="46" spans="1:22">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B46" t="str">
         <f t="shared" si="2"/>
         <v>Integration und Test</v>
@@ -45071,7 +45071,7 @@
         <v>33250</v>
       </c>
     </row>
-    <row r="47" spans="1:22">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B47" t="str">
         <f t="shared" si="2"/>
         <v>Projektmanagement</v>
@@ -45109,7 +45109,7 @@
         <v>-61000</v>
       </c>
     </row>
-    <row r="48" spans="1:22">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B48" t="str">
         <f t="shared" si="2"/>
         <v>Puffer für unerwartetes</v>
@@ -45147,7 +45147,7 @@
         <v>-296400</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B49" t="str">
         <f t="shared" si="2"/>
         <v>Materialkosten</v>
@@ -45185,7 +45185,7 @@
         <v>-4159.9999999999982</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B50" t="str">
         <f>EV[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -45230,7 +45230,7 @@
         <v>-280</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L51" s="2" t="s">
         <v>89</v>
       </c>
@@ -45239,12 +45239,12 @@
         <v>-271510</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="23.25">
+    <row r="53" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A53" s="27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>16</v>
       </c>
@@ -45273,7 +45273,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B56" t="str">
         <f t="shared" ref="B56:B62" si="6">B43</f>
         <v>Anforderungsanalyse</v>
@@ -45317,7 +45317,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B57" t="str">
         <f t="shared" si="6"/>
         <v>Design und Architektur</v>
@@ -45355,7 +45355,7 @@
         <v>-77600</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B58" t="str">
         <f t="shared" si="6"/>
         <v>Implementierung</v>
@@ -45393,7 +45393,7 @@
         <v>-62000</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B59" t="str">
         <f t="shared" si="6"/>
         <v>Integration und Test</v>
@@ -45431,7 +45431,7 @@
         <v>47000</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B60" t="str">
         <f t="shared" si="6"/>
         <v>Projektmanagement</v>
@@ -45469,7 +45469,7 @@
         <v>-11000</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B61" t="str">
         <f t="shared" si="6"/>
         <v>Puffer für unerwartetes</v>
@@ -45507,7 +45507,7 @@
         <v>1200.0000000000073</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B62" t="str">
         <f t="shared" si="6"/>
         <v>Materialkosten</v>
@@ -45552,7 +45552,7 @@
         <v>3320</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B63" t="str">
         <f>CV[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -45597,7 +45597,7 @@
         <v>-125760</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="23.25">
+    <row r="66" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A66" s="27" t="s">
         <v>34</v>
       </c>
@@ -45605,7 +45605,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="68" spans="1:22">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>16</v>
       </c>
@@ -45658,7 +45658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:22">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B69" t="str">
         <f t="shared" ref="B69:B75" si="10">B56</f>
         <v>Anforderungsanalyse</v>
@@ -45728,7 +45728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:22">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B70" t="str">
         <f t="shared" si="10"/>
         <v>Design und Architektur</v>
@@ -45772,7 +45772,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:22">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B71" t="str">
         <f t="shared" si="10"/>
         <v>Implementierung</v>
@@ -45810,7 +45810,7 @@
         <v>2.3058823529411763</v>
       </c>
     </row>
-    <row r="72" spans="1:22">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B72" t="str">
         <f t="shared" si="10"/>
         <v>Integration und Test</v>
@@ -45848,7 +45848,7 @@
         <v>2.1176470588235294</v>
       </c>
     </row>
-    <row r="73" spans="1:22">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B73" t="str">
         <f t="shared" si="10"/>
         <v>Projektmanagement</v>
@@ -45885,7 +45885,7 @@
         <v>0.7009803921568627</v>
       </c>
     </row>
-    <row r="74" spans="1:22">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B74" t="str">
         <f t="shared" si="10"/>
         <v>Puffer für unerwartetes</v>
@@ -45922,7 +45922,7 @@
         <v>0.16176470588235295</v>
       </c>
     </row>
-    <row r="75" spans="1:22">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B75" t="str">
         <f t="shared" si="10"/>
         <v>Materialkosten</v>
@@ -45959,7 +45959,7 @@
         <v>0.74320987654321002</v>
       </c>
     </row>
-    <row r="76" spans="1:22">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B76" t="str">
         <f>SV[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -45997,12 +45997,12 @@
         <v>0.68747050359712225</v>
       </c>
     </row>
-    <row r="79" spans="1:22" ht="23.25">
+    <row r="79" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A79" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>16</v>
       </c>
@@ -46031,7 +46031,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B82" t="str">
         <f t="shared" ref="B82:B88" si="18">B69</f>
         <v>Anforderungsanalyse</v>
@@ -46077,7 +46077,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B83" t="str">
         <f t="shared" si="18"/>
         <v>Design und Architektur</v>
@@ -46121,7 +46121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B84" t="str">
         <f t="shared" si="18"/>
         <v>Implementierung</v>
@@ -46159,7 +46159,7 @@
         <v>0.61250000000000004</v>
       </c>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B85" t="str">
         <f t="shared" si="18"/>
         <v>Integration und Test</v>
@@ -46197,7 +46197,7 @@
         <v>3.9375</v>
       </c>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B86" t="str">
         <f t="shared" si="18"/>
         <v>Projektmanagement</v>
@@ -46234,7 +46234,7 @@
         <v>0.9285714285714286</v>
       </c>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B87" t="str">
         <f t="shared" si="18"/>
         <v>Puffer für unerwartetes</v>
@@ -46271,7 +46271,7 @@
         <v>1.0214285714285716</v>
       </c>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B88" t="str">
         <f t="shared" si="18"/>
         <v>Materialkosten</v>
@@ -46308,7 +46308,7 @@
         <v>0.57333333333333347</v>
       </c>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B89" t="str">
         <f>CPI[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -46346,7 +46346,7 @@
         <v>0.82605809128630703</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="23.25">
+    <row r="92" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A92" s="33" t="s">
         <v>69</v>
       </c>
@@ -46354,17 +46354,17 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="23.25">
+    <row r="94" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A94" s="27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="N95" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>16</v>
       </c>
@@ -46405,7 +46405,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="97" spans="1:18">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B97" t="str">
         <f t="shared" ref="B97:B103" si="26">B82</f>
         <v>Anforderungsanalyse</v>
@@ -46465,7 +46465,7 @@
         <v>14400</v>
       </c>
     </row>
-    <row r="98" spans="1:18">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B98" t="str">
         <f t="shared" si="26"/>
         <v>Design und Architektur</v>
@@ -46519,7 +46519,7 @@
         <v>141600</v>
       </c>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B99" t="str">
         <f t="shared" si="26"/>
         <v>Implementierung</v>
@@ -46573,7 +46573,7 @@
         <v>294000</v>
       </c>
     </row>
-    <row r="100" spans="1:18">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B100" t="str">
         <f t="shared" si="26"/>
         <v>Integration und Test</v>
@@ -46627,7 +46627,7 @@
         <v>189000</v>
       </c>
     </row>
-    <row r="101" spans="1:18">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B101" t="str">
         <f t="shared" si="26"/>
         <v>Projektmanagement</v>
@@ -46681,7 +46681,7 @@
         <v>143000</v>
       </c>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B102" t="str">
         <f t="shared" si="26"/>
         <v>Puffer für unerwartetes</v>
@@ -46735,7 +46735,7 @@
         <v>46799.999999999993</v>
       </c>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B103" t="str">
         <f t="shared" si="26"/>
         <v>Materialkosten</v>
@@ -46789,7 +46789,7 @@
         <v>73960</v>
       </c>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B104" t="str">
         <f>SPI[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -46827,7 +46827,7 @@
         <v>1313.1617942535665</v>
       </c>
     </row>
-    <row r="106" spans="1:18">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="K106" s="2" t="s">
         <v>89</v>
       </c>
@@ -46836,12 +46836,12 @@
         <v>955.91504329004329</v>
       </c>
     </row>
-    <row r="107" spans="1:18" ht="23.25">
+    <row r="107" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A107" s="33" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>16</v>
       </c>
@@ -46870,7 +46870,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="110" spans="1:18">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B110" t="str">
         <f t="shared" ref="B110:C116" si="29">B97</f>
         <v>Anforderungsanalyse</v>
@@ -46914,7 +46914,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B111" t="str">
         <f t="shared" si="29"/>
         <v>Design und Architektur</v>
@@ -46952,7 +46952,7 @@
         <v>218.87499999999997</v>
       </c>
     </row>
-    <row r="112" spans="1:18">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B112" t="str">
         <f t="shared" si="29"/>
         <v>Implementierung</v>
@@ -46990,7 +46990,7 @@
         <v>170.00000000000003</v>
       </c>
     </row>
-    <row r="113" spans="2:13">
+    <row r="113" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B113" t="str">
         <f t="shared" si="29"/>
         <v>Integration und Test</v>
@@ -47028,7 +47028,7 @@
         <v>119.00000000000001</v>
       </c>
     </row>
-    <row r="114" spans="2:13">
+    <row r="114" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B114" t="str">
         <f t="shared" si="29"/>
         <v>Projektmanagement</v>
@@ -47066,7 +47066,7 @@
         <v>408.00000000000006</v>
       </c>
     </row>
-    <row r="115" spans="2:13">
+    <row r="115" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B115" t="str">
         <f t="shared" si="29"/>
         <v>Puffer für unerwartetes</v>
@@ -47104,7 +47104,7 @@
         <v>642.90909090909088</v>
       </c>
     </row>
-    <row r="116" spans="2:13">
+    <row r="116" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B116" t="str">
         <f t="shared" si="29"/>
         <v>Materialkosten</v>
@@ -47142,7 +47142,7 @@
         <v>115.71428571428569</v>
       </c>
     </row>
-    <row r="117" spans="2:13">
+    <row r="117" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B117" t="str">
         <f>ETC[[#Totals],[Posten]]</f>
         <v>Gesamt</v>
@@ -47187,43 +47187,43 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="2:13">
+    <row r="118" spans="2:13" x14ac:dyDescent="0.2">
       <c r="L118">
         <f t="shared" ref="L118:L124" si="30">J111*J70</f>
         <v>235.99999999999997</v>
       </c>
     </row>
-    <row r="119" spans="2:13">
+    <row r="119" spans="2:13" x14ac:dyDescent="0.2">
       <c r="L119">
         <f t="shared" si="30"/>
         <v>392.00000000000006</v>
       </c>
     </row>
-    <row r="120" spans="2:13">
+    <row r="120" spans="2:13" x14ac:dyDescent="0.2">
       <c r="L120">
         <f t="shared" si="30"/>
         <v>252.00000000000003</v>
       </c>
     </row>
-    <row r="121" spans="2:13">
+    <row r="121" spans="2:13" x14ac:dyDescent="0.2">
       <c r="L121">
         <f t="shared" si="30"/>
         <v>286</v>
       </c>
     </row>
-    <row r="122" spans="2:13">
+    <row r="122" spans="2:13" x14ac:dyDescent="0.2">
       <c r="L122">
         <f t="shared" si="30"/>
         <v>104</v>
       </c>
     </row>
-    <row r="123" spans="2:13">
+    <row r="123" spans="2:13" x14ac:dyDescent="0.2">
       <c r="L123">
         <f t="shared" si="30"/>
         <v>86</v>
       </c>
     </row>
-    <row r="124" spans="2:13">
+    <row r="124" spans="2:13" x14ac:dyDescent="0.2">
       <c r="L124">
         <f t="shared" si="30"/>
         <v>1499.9999999999998</v>
@@ -47260,7 +47260,7 @@
       <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
@@ -47269,12 +47269,12 @@
     <col min="10" max="10" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="23.25">
+    <row r="2" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J3" t="s">
         <v>48</v>
       </c>
@@ -47282,7 +47282,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -47311,7 +47311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" t="str">
         <f>Kennzahlen!B56</f>
         <v>Anforderungsanalyse</v>
@@ -47341,7 +47341,7 @@
         <v>POS</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" t="str">
         <f>Kennzahlen!B57</f>
         <v>Design und Architektur</v>
@@ -47377,7 +47377,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" t="str">
         <f>Kennzahlen!B58</f>
         <v>Implementierung</v>
@@ -47413,7 +47413,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" t="str">
         <f>Kennzahlen!B59</f>
         <v>Integration und Test</v>
@@ -47449,7 +47449,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" t="str">
         <f>Kennzahlen!B60</f>
         <v>Projektmanagement</v>
@@ -47479,7 +47479,7 @@
         <v>POS</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" t="str">
         <f>Kennzahlen!B61</f>
         <v>Puffer für unerwartetes</v>
@@ -47515,7 +47515,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" t="str">
         <f>Kennzahlen!B62</f>
         <v>Materialkosten</v>
@@ -47551,7 +47551,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" t="str">
         <f>Kennzahlen!B63</f>
         <v>Gesamt</v>
@@ -47586,7 +47586,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J13" t="s">
         <v>66</v>
       </c>
@@ -47594,12 +47594,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="23.25">
+    <row r="15" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A15" s="27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -47622,7 +47622,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" t="str">
         <f>Kennzahlen!B69</f>
         <v>Anforderungsanalyse</v>
@@ -47648,7 +47648,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" t="str">
         <f>Kennzahlen!B70</f>
         <v>Design und Architektur</v>
@@ -47674,7 +47674,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" t="str">
         <f>Kennzahlen!B71</f>
         <v>Implementierung</v>
@@ -47700,7 +47700,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" t="str">
         <f>Kennzahlen!B72</f>
         <v>Integration und Test</v>
@@ -47726,7 +47726,7 @@
         <v>Grün</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" t="str">
         <f>Kennzahlen!B73</f>
         <v>Projektmanagement</v>
@@ -47752,7 +47752,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" t="str">
         <f>Kennzahlen!B74</f>
         <v>Puffer für unerwartetes</v>
@@ -47778,7 +47778,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" t="str">
         <f>Kennzahlen!B75</f>
         <v>Materialkosten</v>
@@ -47804,7 +47804,7 @@
         <v>Rot</v>
       </c>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" t="str">
         <f>Kennzahlen!B76</f>
         <v>Gesamt</v>
@@ -47897,11 +47897,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="R33" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -47917,7 +47915,7 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
@@ -47932,7 +47930,7 @@
     <col min="16" max="16" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="12.95" customHeight="1">
+    <row r="1" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -47983,7 +47981,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="12.95" customHeight="1">
+    <row r="2" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -48039,7 +48037,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12.95" customHeight="1">
+    <row r="3" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -48095,7 +48093,7 @@
         <v>0.15733333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.95" customHeight="1">
+    <row r="4" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -48151,7 +48149,7 @@
         <v>0.26133333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="12.95" customHeight="1">
+    <row r="5" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -48207,7 +48205,7 @@
         <v>0.16800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="12.95" customHeight="1">
+    <row r="6" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -48263,7 +48261,7 @@
         <v>0.19066666666666668</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="12.95" customHeight="1">
+    <row r="7" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -48319,7 +48317,7 @@
         <v>6.933333333333333E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" ht="12.95" customHeight="1">
+    <row r="8" spans="1:17" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -48384,11 +48382,11 @@
         <v>1414000</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="12.95" customHeight="1">
+    <row r="9" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="P9" s="10"/>
     </row>
-    <row r="10" spans="1:17" ht="12.95" customHeight="1">
+    <row r="10" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
@@ -48449,7 +48447,7 @@
       </c>
       <c r="P10" s="10"/>
     </row>
-    <row r="11" spans="1:17" ht="12.95" customHeight="1">
+    <row r="11" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
@@ -48505,7 +48503,7 @@
         <v>5.7333333333333333E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="2" customFormat="1" ht="12.95" customHeight="1">
+    <row r="12" spans="1:17" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -48563,7 +48561,7 @@
       </c>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:17" ht="12.95" customHeight="1">
+    <row r="13" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -48578,7 +48576,7 @@
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
     </row>
-    <row r="14" spans="1:17" ht="12.95" customHeight="1">
+    <row r="14" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
@@ -48601,12 +48599,12 @@
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
     </row>
-    <row r="17" spans="1:16" ht="12.95" customHeight="1">
+    <row r="17" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="12.95" customHeight="1">
+    <row r="18" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -48652,7 +48650,7 @@
       <c r="O18" s="2"/>
       <c r="P18" s="3"/>
     </row>
-    <row r="19" spans="1:16" ht="12.95" customHeight="1">
+    <row r="19" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>1</v>
       </c>
@@ -48711,7 +48709,7 @@
       <c r="O19" s="6"/>
       <c r="P19" s="7"/>
     </row>
-    <row r="20" spans="1:16" ht="12.95" customHeight="1">
+    <row r="20" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>2</v>
       </c>
@@ -48770,7 +48768,7 @@
       <c r="O20" s="6"/>
       <c r="P20" s="7"/>
     </row>
-    <row r="21" spans="1:16" ht="12.95" customHeight="1">
+    <row r="21" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>3</v>
       </c>
@@ -48829,7 +48827,7 @@
       <c r="O21" s="6"/>
       <c r="P21" s="7"/>
     </row>
-    <row r="22" spans="1:16" ht="12.95" customHeight="1">
+    <row r="22" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
@@ -48888,7 +48886,7 @@
       <c r="O22" s="6"/>
       <c r="P22" s="7"/>
     </row>
-    <row r="23" spans="1:16" ht="12.95" customHeight="1">
+    <row r="23" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -48947,7 +48945,7 @@
       <c r="O23" s="6"/>
       <c r="P23" s="7"/>
     </row>
-    <row r="24" spans="1:16" ht="12.95" customHeight="1">
+    <row r="24" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>6</v>
       </c>
@@ -49006,7 +49004,7 @@
       <c r="O24" s="6"/>
       <c r="P24" s="7"/>
     </row>
-    <row r="25" spans="1:16" ht="12.95" customHeight="1">
+    <row r="25" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
@@ -49065,7 +49063,7 @@
       <c r="O25" s="2"/>
       <c r="P25" s="8"/>
     </row>
-    <row r="26" spans="1:16" s="2" customFormat="1" ht="12.95" customHeight="1">
+    <row r="26" spans="1:16" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="37" t="s">
         <v>80</v>
       </c>
@@ -49138,7 +49136,7 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="8" width="9.42578125" customWidth="1"/>
@@ -49150,7 +49148,7 @@
     <col min="16" max="16" width="12.28515625" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="12.95" customHeight="1">
+    <row r="1" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -49182,7 +49180,7 @@
       <c r="O1" s="22"/>
       <c r="P1" s="23"/>
     </row>
-    <row r="2" spans="1:16" ht="12.95" customHeight="1">
+    <row r="2" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
@@ -49208,7 +49206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="12.95" customHeight="1">
+    <row r="3" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
@@ -49234,7 +49232,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="12.95" customHeight="1">
+    <row r="4" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
@@ -49260,7 +49258,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="12.95" customHeight="1">
+    <row r="5" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
@@ -49286,7 +49284,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12.95" customHeight="1">
+    <row r="6" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
@@ -49312,7 +49310,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="12.95" customHeight="1">
+    <row r="7" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
@@ -49338,7 +49336,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="12.95" customHeight="1">
+    <row r="8" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
         <f>'Budgetierte Kosten'!A8</f>
         <v>Summe Personenstunden pro Monat</v>
@@ -49372,7 +49370,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="12.95" customHeight="1">
+    <row r="9" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -49382,7 +49380,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="12.95" customHeight="1">
+    <row r="10" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -49415,7 +49413,7 @@
         <v>80750</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="12.95" customHeight="1">
+    <row r="11" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -49449,7 +49447,7 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
     </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" ht="12.95" customHeight="1">
+    <row r="12" spans="1:16" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -49490,7 +49488,7 @@
       <c r="O12" s="24"/>
       <c r="P12" s="25"/>
     </row>
-    <row r="15" spans="1:16" ht="12.95" customHeight="1">
+    <row r="15" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -49514,7 +49512,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="3" width="10.140625" customWidth="1"/>
@@ -49523,7 +49521,7 @@
     <col min="12" max="13" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.95" customHeight="1">
+    <row r="1" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -49554,7 +49552,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" ht="12.95" customHeight="1">
+    <row r="2" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="str">
         <f>'Budgetierte Kosten'!A2</f>
         <v>Anforderungsanalyse</v>
@@ -49581,7 +49579,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.95" customHeight="1">
+    <row r="3" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="str">
         <f>'Budgetierte Kosten'!A3</f>
         <v>Design und Architektur</v>
@@ -49608,7 +49606,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.95" customHeight="1">
+    <row r="4" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="str">
         <f>'Budgetierte Kosten'!A4</f>
         <v>Implementierung</v>
@@ -49635,7 +49633,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.95" customHeight="1">
+    <row r="5" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="str">
         <f>'Budgetierte Kosten'!A5</f>
         <v>Integration und Test</v>
@@ -49662,7 +49660,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.95" customHeight="1">
+    <row r="6" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="str">
         <f>'Budgetierte Kosten'!A6</f>
         <v>Projektmanagement</v>
@@ -49689,7 +49687,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.95" customHeight="1">
+    <row r="7" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="str">
         <f>'Budgetierte Kosten'!A7</f>
         <v>Puffer für unerwartetes</v>
@@ -49716,7 +49714,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.95" customHeight="1">
+    <row r="8" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -49747,7 +49745,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="12.95" customHeight="1">
+    <row r="9" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
@@ -49761,7 +49759,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" ht="12.95" customHeight="1">
+    <row r="10" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
@@ -49775,12 +49773,12 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" ht="12.95" customHeight="1">
+    <row r="11" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.95" customHeight="1">
+    <row r="12" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -49806,7 +49804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="12.95" customHeight="1">
+    <row r="13" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="str">
         <f>'Budgetierte Kosten'!A2</f>
         <v>Anforderungsanalyse</v>
@@ -49840,7 +49838,7 @@
         <v>8.6400000000000005E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="12.95" customHeight="1">
+    <row r="14" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="str">
         <f>'Budgetierte Kosten'!A3</f>
         <v>Design und Architektur</v>
@@ -49874,7 +49872,7 @@
         <v>6.2933333333333327E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="12.95" customHeight="1">
+    <row r="15" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="str">
         <f>'Budgetierte Kosten'!A4</f>
         <v>Implementierung</v>
@@ -49908,7 +49906,7 @@
         <v>6.5333333333333327E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="12.95" customHeight="1">
+    <row r="16" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="str">
         <f>'Budgetierte Kosten'!A5</f>
         <v>Integration und Test</v>
@@ -49942,7 +49940,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="12.95" customHeight="1">
+    <row r="17" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="str">
         <f>'Budgetierte Kosten'!A6</f>
         <v>Projektmanagement</v>
@@ -49976,7 +49974,7 @@
         <v>9.5333333333333339E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="12.95" customHeight="1">
+    <row r="18" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="str">
         <f>'Budgetierte Kosten'!A7</f>
         <v>Puffer für unerwartetes</v>
@@ -50010,7 +50008,7 @@
         <v>3.8133333333333332E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="12.95" customHeight="1">
+    <row r="19" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -50043,7 +50041,7 @@
         <v>8.0266666666666681E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="12.95" customHeight="1">
+    <row r="20" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Gesamtbudget zu Diagrammen hinzugefügt + Icon angepasst
</commit_message>
<xml_diff>
--- a/Lab1/Auswertung Final.xlsx
+++ b/Lab1/Auswertung Final.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sack\Christian\A\Studium\4 - Semester\SpBC\Übungen\swpbc\Lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\Dropbox\033 534 - Bachelorstudium Software &amp; Information Engineering\__LVAs\Softwareprojekt-Beobachtung und -Controlling\GIT repo\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="10950" tabRatio="587" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Kennzahlen" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="94">
   <si>
     <t>Aktivität / Monat</t>
   </si>
@@ -304,18 +304,21 @@
   <si>
     <t>(obsolet)</t>
   </si>
+  <si>
+    <t>Gesamtbudget</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0;\-&quot;€&quot;\ #,##0"/>
-    <numFmt numFmtId="165" formatCode="&quot;€ &quot;#,##0"/>
-    <numFmt numFmtId="166" formatCode="&quot;€ &quot;#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="168" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="5" formatCode="&quot;€&quot;\ #,##0;\-&quot;€&quot;\ #,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;€ &quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;€ &quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="167" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -561,7 +564,7 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -569,28 +572,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -605,8 +608,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="5" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Accent" xfId="13"/>
@@ -628,51 +632,6 @@
     <cellStyle name="Warning" xfId="11"/>
   </cellStyles>
   <dxfs count="159">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -749,6 +708,51 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -889,226 +893,226 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0\ &quot;€&quot;"/>
+      <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     </dxf>
     <dxf>
       <fill>
@@ -11852,6 +11856,106 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Budgetierte Kosten'!$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gesamtbudget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Budgetierte Kosten'!$A$30:$H$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Budgetierte Kosten'!$B$29:$I$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A158-452A-9C51-272FF5CE6546}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -12112,10 +12216,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.78122258819490042"/>
-          <c:y val="0.15941065313967398"/>
-          <c:w val="0.19300011049188981"/>
-          <c:h val="0.26460376464234242"/>
+          <c:x val="0.77898369407736534"/>
+          <c:y val="0.16637090351967329"/>
+          <c:w val="0.21863596134620294"/>
+          <c:h val="0.4008102716152801"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -12376,7 +12480,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$19:$N$19</c:f>
               <c:numCache>
-                <c:formatCode>"€"\ #,##0;\-"€"\ #,##0</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>48000</c:v>
@@ -12454,7 +12558,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$20:$N$20</c:f>
               <c:numCache>
-                <c:formatCode>"€"\ #,##0;\-"€"\ #,##0</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -12532,7 +12636,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$21:$N$21</c:f>
               <c:numCache>
-                <c:formatCode>"€"\ #,##0;\-"€"\ #,##0</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -12610,7 +12714,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$22:$N$22</c:f>
               <c:numCache>
-                <c:formatCode>"€"\ #,##0;\-"€"\ #,##0</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -12688,7 +12792,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$23:$N$23</c:f>
               <c:numCache>
-                <c:formatCode>"€"\ #,##0;\-"€"\ #,##0</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>22000</c:v>
@@ -12768,7 +12872,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$24:$N$24</c:f>
               <c:numCache>
-                <c:formatCode>"€"\ #,##0;\-"€"\ #,##0</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>8000</c:v>
@@ -12848,7 +12952,7 @@
             <c:numRef>
               <c:f>'Budgetierte Kosten'!$B$25:$N$25</c:f>
               <c:numCache>
-                <c:formatCode>"€"\ #,##0;\-"€"\ #,##0</c:formatCode>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
@@ -12911,6 +13015,106 @@
         <c:axId val="363063576"/>
         <c:axId val="363062264"/>
       </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Budgetierte Kosten'!$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gesamtbudget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Budgetierte Kosten'!$B$28:$N$28</c:f>
+              <c:numCache>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1250000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FEBA-4051-BF79-BDCC6EABBCCA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="363063576"/>
+        <c:axId val="363062264"/>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="363063576"/>
         <c:scaling>
@@ -13154,8 +13358,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.81143317805227955"/>
           <c:y val="9.756720357962588E-2"/>
-          <c:w val="0.17814270398610335"/>
-          <c:h val="0.37871547765859387"/>
+          <c:w val="0.18856687265508662"/>
+          <c:h val="0.47890611848446424"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -42900,7 +43104,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="EAC" displayName="EAC" ref="B109:J117" totalsRowCount="1">
   <autoFilter ref="B109:J116"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="14">
+    <tableColumn id="1" name="Posten" totalsRowFunction="custom" dataDxfId="31">
       <calculatedColumnFormula>B97</calculatedColumnFormula>
       <totalsRowFormula>ETC[[#Totals],[Posten]]</totalsRowFormula>
     </tableColumn>
@@ -42908,31 +43112,31 @@
       <calculatedColumnFormula>C97</calculatedColumnFormula>
       <totalsRowFormula>ETC[[#Totals],[0 '[k €']]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="1 [k €]" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="2" name="1 [k €]" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="29">
       <calculatedColumnFormula>IF(D69=$M$70,$M$70,'Budgetierte Kosten'!$P2/(D69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[1]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="2 [k €]" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="3" name="2 [k €]" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="27">
       <calculatedColumnFormula>IF(E69=$M$70,$M$70,$E$92/(E69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[2]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="3 [k €]" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="4" name="3 [k €]" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="25">
       <calculatedColumnFormula>IF(F69=$M$70,$M$70,$E$92/(F69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[3]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="4 [k €]" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="5" name="4 [k €]" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="23">
       <calculatedColumnFormula>IF(G69=$M$70,$M$70,$E$92/(G69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[4]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="5 [k €]" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="6" name="5 [k €]" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="21">
       <calculatedColumnFormula>IF(H69=$M$70,$M$70,$E$92/(H69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[5]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="6 [k €]" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="7" name="6 [k €]" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="19">
       <calculatedColumnFormula>IF(I69=$M$70,$M$70,$E$92/(I69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[6]]*1000)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="7 [k €]" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="8" name="7 [k €]" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="17">
       <calculatedColumnFormula>IF(J69=$M$70,$M$70,$E$92/(J69*1000))</calculatedColumnFormula>
       <totalsRowFormula>$E$92/(CPI[[#Totals],[7]]*1000)</totalsRowFormula>
     </tableColumn>
@@ -42965,20 +43169,20 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B56</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="25">
+    <tableColumn id="2" name="CPI" dataDxfId="10">
       <calculatedColumnFormula>Kennzahlen!J69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="24">
+    <tableColumn id="3" name="SPI" dataDxfId="9">
       <calculatedColumnFormula>Kennzahlen!J82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="23">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="8">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="22"/>
-    <tableColumn id="6" name="Status" dataDxfId="21">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="7"/>
+    <tableColumn id="6" name="Status" dataDxfId="6">
       <calculatedColumnFormula>IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$3, Tabelle9[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;$K$4, Tabelle9[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Trend" dataDxfId="20">
+    <tableColumn id="7" name="Trend" dataDxfId="5">
       <calculatedColumnFormula>IF(C18=Kennzahlen!$M$70,Kennzahlen!$M$70,IF(OR(ABS(Tabelle9[[#This Row],[CPI]]-C18)&lt;=$K$13),$K$12, IF(OR(Tabelle9[[#This Row],[CPI]]&lt;C18,Tabelle9[[#This Row],[SPI]]&lt;D18), $K$11, $K$10)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -42993,19 +43197,19 @@
     <tableColumn id="1" name="Posten">
       <calculatedColumnFormula>Kennzahlen!B69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="CPI" dataDxfId="19">
+    <tableColumn id="2" name="CPI" dataDxfId="4">
       <calculatedColumnFormula>Kennzahlen!I69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SPI" dataDxfId="18">
+    <tableColumn id="3" name="SPI" dataDxfId="3">
       <calculatedColumnFormula>Kennzahlen!I82</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Abgeschlossen" dataDxfId="17">
+    <tableColumn id="4" name="Abgeschlossen" dataDxfId="2">
       <calculatedColumnFormula>'Fertigstellungsgrad der Akt.'!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Budget [k €]" dataDxfId="16">
+    <tableColumn id="5" name="Budget [k €]" dataDxfId="1">
       <calculatedColumnFormula>F5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Status" dataDxfId="15">
+    <tableColumn id="6" name="Status" dataDxfId="0">
       <calculatedColumnFormula>IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$3, Tabelle911[[#This Row],[SPI]]&lt;$K$3),$K$6, IF(OR(Tabelle911[[#This Row],[CPI]]&lt;$K$4, Tabelle911[[#This Row],[SPI]]&lt;$K$4),$K$7, $K$8))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Trend"/>
@@ -43743,8 +43947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N105" sqref="N105"/>
+    <sheetView topLeftCell="A66" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -47838,13 +48042,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:D12 C18:D25">
-    <cfRule type="cellIs" dxfId="31" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="greaterThanOrEqual">
       <formula>$K$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="lessThan">
       <formula>$K$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
       <formula>$K$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47903,8 +48107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I138" sqref="I138"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M139" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="U162" sqref="U162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -47917,23 +48121,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="2" max="14" width="11.42578125" customWidth="1"/>
     <col min="15" max="15" width="15.42578125" customWidth="1"/>
     <col min="16" max="16" width="14.85546875" customWidth="1"/>
   </cols>
@@ -49126,6 +49323,151 @@
       <c r="N26" s="40">
         <f t="shared" si="10"/>
         <v>1500000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="37"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="40"/>
+      <c r="N27" s="40"/>
+    </row>
+    <row r="28" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="39">
+        <v>1250000</v>
+      </c>
+      <c r="C28" s="39">
+        <v>1250000</v>
+      </c>
+      <c r="D28" s="39">
+        <v>1250000</v>
+      </c>
+      <c r="E28" s="39">
+        <v>1250000</v>
+      </c>
+      <c r="F28" s="39">
+        <v>1250000</v>
+      </c>
+      <c r="G28" s="39">
+        <v>1250000</v>
+      </c>
+      <c r="H28" s="39">
+        <v>1250000</v>
+      </c>
+      <c r="I28" s="39">
+        <v>1250000</v>
+      </c>
+      <c r="J28" s="39">
+        <v>1250000</v>
+      </c>
+      <c r="K28" s="39">
+        <v>1250000</v>
+      </c>
+      <c r="L28" s="39">
+        <v>1250000</v>
+      </c>
+      <c r="M28" s="39">
+        <v>1250000</v>
+      </c>
+      <c r="N28" s="39">
+        <v>1250000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>1250</v>
+      </c>
+      <c r="C29">
+        <v>1250</v>
+      </c>
+      <c r="D29">
+        <v>1250</v>
+      </c>
+      <c r="E29">
+        <v>1250</v>
+      </c>
+      <c r="F29">
+        <v>1250</v>
+      </c>
+      <c r="G29">
+        <v>1250</v>
+      </c>
+      <c r="H29">
+        <v>1250</v>
+      </c>
+      <c r="I29">
+        <v>1250</v>
+      </c>
+      <c r="J29">
+        <v>1250</v>
+      </c>
+      <c r="K29">
+        <v>1250</v>
+      </c>
+      <c r="L29">
+        <v>1250</v>
+      </c>
+      <c r="M29">
+        <v>1250</v>
+      </c>
+      <c r="N29">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>6</v>
+      </c>
+      <c r="H30">
+        <v>7</v>
+      </c>
+      <c r="I30">
+        <v>8</v>
+      </c>
+      <c r="J30">
+        <v>9</v>
+      </c>
+      <c r="K30">
+        <v>10</v>
+      </c>
+      <c r="L30">
+        <v>11</v>
+      </c>
+      <c r="M30">
+        <v>12</v>
+      </c>
+      <c r="N30">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>